<commit_message>
pageinsight flow pushed by Manik on 15.11.2018.20.24
</commit_message>
<xml_diff>
--- a/data/Performance_Audit.xlsx
+++ b/data/Performance_Audit.xlsx
@@ -4,12 +4,12 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView activeTab="2" windowHeight="4305" windowWidth="14640"/>
+    <workbookView windowWidth="14640" windowHeight="4305" activeTab="2"/>
   </bookViews>
   <sheets>
-    <sheet name="Web_Page_Test_Mobile" r:id="rId1" sheetId="1"/>
-    <sheet name="Web_Page_Test_Desktop" r:id="rId2" sheetId="2"/>
-    <sheet name="Page_Insight" r:id="rId3" sheetId="3"/>
+    <sheet name="Web_Page_Test_Mobile" sheetId="1" r:id="rId1"/>
+    <sheet name="Web_Page_Test_Desktop" sheetId="2" r:id="rId2"/>
+    <sheet name="Page_Insight" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="144525"/>
   <oleSize ref="A1:C11"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80">
   <si>
     <t>Urls</t>
   </si>
@@ -257,42 +257,6 @@
   </si>
   <si>
     <t/>
-  </si>
-  <si>
-    <t>43</t>
-  </si>
-  <si>
-    <t>98</t>
-  </si>
-  <si>
-    <t>81</t>
-  </si>
-  <si>
-    <t>95</t>
-  </si>
-  <si>
-    <t>82</t>
-  </si>
-  <si>
-    <t>97</t>
-  </si>
-  <si>
-    <t>20</t>
-  </si>
-  <si>
-    <t>16</t>
-  </si>
-  <si>
-    <t>68</t>
-  </si>
-  <si>
-    <t>90</t>
-  </si>
-  <si>
-    <t>100</t>
-  </si>
-  <si>
-    <t>42</t>
   </si>
 </sst>
 </file>
@@ -300,10 +264,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="_ &quot;₹&quot;\ * #,##0_ ;_ &quot;₹&quot;\ * \-#,##0_ ;_ &quot;₹&quot;\ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;\ * #,##0.00_ ;_ &quot;₹&quot;\ * \-#,##0.00_ ;_ &quot;₹&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ &quot;₹&quot;\ * #,##0_ ;_ &quot;₹&quot;\ * \-#,##0_ ;_ &quot;₹&quot;\ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_ &quot;₹&quot;\ * #,##0.00_ ;_ &quot;₹&quot;\ * \-#,##0.00_ ;_ &quot;₹&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="23">
     <font>
@@ -334,6 +298,126 @@
       <charset val="134"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color theme="1"/>
@@ -344,81 +428,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -431,52 +441,6 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="35">
     <fill>
@@ -499,31 +463,175 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -535,151 +643,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -723,32 +687,6 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
       <top/>
       <bottom style="medium">
         <color theme="4"/>
@@ -771,20 +709,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -800,6 +735,35 @@
       </top>
       <bottom style="thin">
         <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -820,232 +784,232 @@
     </border>
   </borders>
   <cellStyleXfs count="49">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="12" fontId="14" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="0" numFmtId="176">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="0" numFmtId="177">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="0" numFmtId="178">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="0" numFmtId="179">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="0" numFmtId="9">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyNumberFormat="0" applyProtection="0" borderId="6" fillId="5" fontId="7" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="5" fillId="0" fontId="6" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyFont="0" applyNumberFormat="0" applyProtection="0" borderId="9" fillId="13" fontId="0" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="19" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="18" fontId="17" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="22" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="21" fontId="14" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="10" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="26" fontId="14" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="18" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="13" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="5" fillId="0" fontId="16" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="7" fillId="0" fontId="12" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="12" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyNumberFormat="0" applyProtection="0" borderId="4" fillId="7" fontId="9" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="17" fontId="17" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="8" fontId="11" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyNumberFormat="0" applyProtection="0" borderId="10" fillId="4" fontId="21" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="28" fontId="14" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyNumberFormat="0" applyProtection="0" borderId="4" fillId="4" fontId="5" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="8" fillId="0" fontId="15" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="3" fillId="0" fontId="4" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="6" fontId="8" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="19" fontId="20" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="14" fontId="17" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="11" fontId="14" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="27" fontId="17" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="31" fontId="17" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="10" fontId="14" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="33" fontId="14" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="32" fontId="17" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="20" fontId="17" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="34" fontId="14" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="30" fontId="17" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="25" fontId="14" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="9" fontId="14" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="24" fontId="17" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="16" fontId="14" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="23" fontId="17" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="15" fontId="17" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="22" fontId="14" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="29" fontId="17" numFmtId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="11" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
   <cellXfs count="8">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="1" fillId="2" fontId="1" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="2" fillId="3" fontId="2" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf applyBorder="1" borderId="2" fillId="0" fontId="0" numFmtId="0" xfId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="2" fillId="0" fontId="3" numFmtId="9" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="2" fillId="3" fontId="3" numFmtId="9" xfId="0">
+    <xf numFmtId="9" fontId="3" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" borderId="2" fillId="0" fontId="0" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="2" fillId="2" fontId="1" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
-    <cellStyle builtinId="31" name="40% - Accent1" xfId="1"/>
-    <cellStyle builtinId="3" name="Comma" xfId="2"/>
-    <cellStyle builtinId="6" name="Comma [0]" xfId="3"/>
-    <cellStyle builtinId="7" name="Currency [0]" xfId="4"/>
-    <cellStyle builtinId="4" name="Currency" xfId="5"/>
-    <cellStyle builtinId="5" name="Percent" xfId="6"/>
-    <cellStyle builtinId="23" name="Check Cell" xfId="7"/>
-    <cellStyle builtinId="17" name="Heading 2" xfId="8"/>
-    <cellStyle builtinId="10" name="Note" xfId="9"/>
-    <cellStyle builtinId="8" name="Hyperlink" xfId="10"/>
-    <cellStyle builtinId="44" name="60% - Accent4" xfId="11"/>
-    <cellStyle builtinId="9" name="Followed Hyperlink" xfId="12"/>
-    <cellStyle builtinId="39" name="40% - Accent3" xfId="13"/>
-    <cellStyle builtinId="11" name="Warning Text" xfId="14"/>
-    <cellStyle builtinId="35" name="40% - Accent2" xfId="15"/>
-    <cellStyle builtinId="15" name="Title" xfId="16"/>
-    <cellStyle builtinId="53" name="CExplanatory Text" xfId="17"/>
-    <cellStyle builtinId="16" name="Heading 1" xfId="18"/>
-    <cellStyle builtinId="18" name="Heading 3" xfId="19"/>
-    <cellStyle builtinId="19" name="Heading 4" xfId="20"/>
-    <cellStyle builtinId="20" name="Input" xfId="21"/>
-    <cellStyle builtinId="40" name="60% - Accent3" xfId="22"/>
-    <cellStyle builtinId="26" name="Good" xfId="23"/>
-    <cellStyle builtinId="21" name="Output" xfId="24"/>
-    <cellStyle builtinId="30" name="20% - Accent1" xfId="25"/>
-    <cellStyle builtinId="22" name="Calculation" xfId="26"/>
-    <cellStyle builtinId="24" name="Linked Cell" xfId="27"/>
-    <cellStyle builtinId="25" name="Total" xfId="28"/>
-    <cellStyle builtinId="27" name="Bad" xfId="29"/>
-    <cellStyle builtinId="28" name="Neutral" xfId="30"/>
-    <cellStyle builtinId="29" name="Accent1" xfId="31"/>
-    <cellStyle builtinId="46" name="20% - Accent5" xfId="32"/>
-    <cellStyle builtinId="32" name="60% - Accent1" xfId="33"/>
-    <cellStyle builtinId="33" name="Accent2" xfId="34"/>
-    <cellStyle builtinId="34" name="20% - Accent2" xfId="35"/>
-    <cellStyle builtinId="50" name="20% - Accent6" xfId="36"/>
-    <cellStyle builtinId="36" name="60% - Accent2" xfId="37"/>
-    <cellStyle builtinId="37" name="Accent3" xfId="38"/>
-    <cellStyle builtinId="38" name="20% - Accent3" xfId="39"/>
-    <cellStyle builtinId="41" name="Accent4" xfId="40"/>
-    <cellStyle builtinId="42" name="20% - Accent4" xfId="41"/>
-    <cellStyle builtinId="43" name="40% - Accent4" xfId="42"/>
-    <cellStyle builtinId="45" name="Accent5" xfId="43"/>
-    <cellStyle builtinId="47" name="40% - Accent5" xfId="44"/>
-    <cellStyle builtinId="48" name="60% - Accent5" xfId="45"/>
-    <cellStyle builtinId="49" name="Accent6" xfId="46"/>
-    <cellStyle builtinId="51" name="40% - Accent6" xfId="47"/>
-    <cellStyle builtinId="52" name="60% - Accent6" xfId="48"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="40% - Accent1" xfId="1" builtinId="31"/>
+    <cellStyle name="Comma" xfId="2" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="3" builtinId="6"/>
+    <cellStyle name="Currency [0]" xfId="4" builtinId="7"/>
+    <cellStyle name="Currency" xfId="5" builtinId="4"/>
+    <cellStyle name="Percent" xfId="6" builtinId="5"/>
+    <cellStyle name="Check Cell" xfId="7" builtinId="23"/>
+    <cellStyle name="Heading 2" xfId="8" builtinId="17"/>
+    <cellStyle name="Note" xfId="9" builtinId="10"/>
+    <cellStyle name="Hyperlink" xfId="10" builtinId="8"/>
+    <cellStyle name="60% - Accent4" xfId="11" builtinId="44"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9"/>
+    <cellStyle name="40% - Accent3" xfId="13" builtinId="39"/>
+    <cellStyle name="Warning Text" xfId="14" builtinId="11"/>
+    <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
+    <cellStyle name="Title" xfId="16" builtinId="15"/>
+    <cellStyle name="CExplanatory Text" xfId="17" builtinId="53"/>
+    <cellStyle name="Heading 1" xfId="18" builtinId="16"/>
+    <cellStyle name="Heading 3" xfId="19" builtinId="18"/>
+    <cellStyle name="Heading 4" xfId="20" builtinId="19"/>
+    <cellStyle name="Input" xfId="21" builtinId="20"/>
+    <cellStyle name="60% - Accent3" xfId="22" builtinId="40"/>
+    <cellStyle name="Good" xfId="23" builtinId="26"/>
+    <cellStyle name="Output" xfId="24" builtinId="21"/>
+    <cellStyle name="20% - Accent1" xfId="25" builtinId="30"/>
+    <cellStyle name="Calculation" xfId="26" builtinId="22"/>
+    <cellStyle name="Linked Cell" xfId="27" builtinId="24"/>
+    <cellStyle name="Total" xfId="28" builtinId="25"/>
+    <cellStyle name="Bad" xfId="29" builtinId="27"/>
+    <cellStyle name="Neutral" xfId="30" builtinId="28"/>
+    <cellStyle name="Accent1" xfId="31" builtinId="29"/>
+    <cellStyle name="20% - Accent5" xfId="32" builtinId="46"/>
+    <cellStyle name="60% - Accent1" xfId="33" builtinId="32"/>
+    <cellStyle name="Accent2" xfId="34" builtinId="33"/>
+    <cellStyle name="20% - Accent2" xfId="35" builtinId="34"/>
+    <cellStyle name="20% - Accent6" xfId="36" builtinId="50"/>
+    <cellStyle name="60% - Accent2" xfId="37" builtinId="36"/>
+    <cellStyle name="Accent3" xfId="38" builtinId="37"/>
+    <cellStyle name="20% - Accent3" xfId="39" builtinId="38"/>
+    <cellStyle name="Accent4" xfId="40" builtinId="41"/>
+    <cellStyle name="20% - Accent4" xfId="41" builtinId="42"/>
+    <cellStyle name="40% - Accent4" xfId="42" builtinId="43"/>
+    <cellStyle name="Accent5" xfId="43" builtinId="45"/>
+    <cellStyle name="40% - Accent5" xfId="44" builtinId="47"/>
+    <cellStyle name="60% - Accent5" xfId="45" builtinId="48"/>
+    <cellStyle name="Accent6" xfId="46" builtinId="49"/>
+    <cellStyle name="40% - Accent6" xfId="47" builtinId="51"/>
+    <cellStyle name="60% - Accent6" xfId="48" builtinId="52"/>
   </cellStyles>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -1059,10 +1023,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -1226,21 +1190,21 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="6350">
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="12700">
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="19050">
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -1257,7 +1221,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw algn="ctr" blurRad="57150" dir="5400000" dist="19050" rotWithShape="0">
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -1310,9 +1274,9 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1320,12 +1284,12 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="2"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="34.2857142857143" collapsed="false"/>
-    <col min="2" max="2" customWidth="true" width="21.2857142857143" collapsed="false"/>
-    <col min="3" max="3" customWidth="true" width="80.8571428571429" collapsed="false"/>
+    <col min="1" max="1" width="34.2857142857143" customWidth="1"/>
+    <col min="2" max="2" width="21.2857142857143" customWidth="1"/>
+    <col min="3" max="3" width="80.8571428571429" customWidth="1"/>
   </cols>
   <sheetData>
-    <row ht="30" r="1" spans="1:3">
+    <row r="1" ht="30" spans="1:3">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -1447,15 +1411,15 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.511805555555556" header="0.511805555555556" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
   <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B18" sqref="B18"/>
@@ -1463,14 +1427,14 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="4"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="37.5714285714286" collapsed="false"/>
-    <col min="2" max="2" customWidth="true" width="9.85714285714286" collapsed="false"/>
-    <col min="3" max="3" customWidth="true" width="8.85714285714286" collapsed="false"/>
-    <col min="4" max="4" customWidth="true" width="14.0" collapsed="false"/>
-    <col min="5" max="5" customWidth="true" width="89.2857142857143" collapsed="false"/>
+    <col min="1" max="1" width="37.5714285714286" customWidth="1"/>
+    <col min="2" max="2" width="9.85714285714286" customWidth="1"/>
+    <col min="3" max="3" width="8.85714285714286" customWidth="1"/>
+    <col min="4" max="4" width="14" customWidth="1"/>
+    <col min="5" max="5" width="89.2857142857143" customWidth="1"/>
   </cols>
   <sheetData>
-    <row ht="30" r="1" spans="1:5">
+    <row r="1" ht="30" spans="1:5">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -1658,24 +1622,24 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.511805555555556" header="0.511805555555556" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
   <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B2" sqref="B2:C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="3" outlineLevelRow="7"/>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="7" outlineLevelCol="3"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="37.5714285714286" collapsed="false"/>
-    <col min="3" max="3" customWidth="true" width="12.2857142857143" collapsed="false"/>
+    <col min="1" max="1" width="37.5714285714286" customWidth="1"/>
+    <col min="3" max="3" width="12.2857142857143" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -1693,12 +1657,8 @@
       <c r="A2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>81</v>
-      </c>
+      <c r="B2" s="3"/>
+      <c r="C2" s="3"/>
       <c r="D2" t="s">
         <v>79</v>
       </c>
@@ -1707,12 +1667,8 @@
       <c r="A3" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>83</v>
-      </c>
+      <c r="B3" s="4"/>
+      <c r="C3" s="4"/>
       <c r="D3" t="s">
         <v>79</v>
       </c>
@@ -1721,59 +1677,39 @@
       <c r="A4" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>85</v>
-      </c>
+      <c r="B4" s="4"/>
+      <c r="C4" s="4"/>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B5" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>82</v>
-      </c>
+      <c r="B5" s="4"/>
+      <c r="C5" s="4"/>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B6" s="5" t="s">
-        <v>87</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>88</v>
-      </c>
+      <c r="B6" s="5"/>
+      <c r="C6" s="4"/>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B7" s="6" t="s">
-        <v>89</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>90</v>
-      </c>
+      <c r="B7" s="6"/>
+      <c r="C7" s="6"/>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="B8" s="6" t="s">
-        <v>91</v>
-      </c>
-      <c r="C8" s="6" t="s">
-        <v>83</v>
-      </c>
+      <c r="B8" s="6"/>
+      <c r="C8" s="6"/>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.511805555555556" header="0.511805555555556" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
   <headerFooter/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Committed on 16:11:2018:15:30:00PM By Karthikeyan Rajendran
</commit_message>
<xml_diff>
--- a/data/Performance_Audit.xlsx
+++ b/data/Performance_Audit.xlsx
@@ -4,12 +4,12 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="14640" windowHeight="4305" activeTab="2"/>
+    <workbookView activeTab="2" windowHeight="8370" windowWidth="20385"/>
   </bookViews>
   <sheets>
-    <sheet name="Web_Page_Test_Mobile" sheetId="1" r:id="rId1"/>
-    <sheet name="Web_Page_Test_Desktop" sheetId="2" r:id="rId2"/>
-    <sheet name="Page_Insight" sheetId="3" r:id="rId3"/>
+    <sheet name="Web_Page_Test_Mobile" r:id="rId1" sheetId="1"/>
+    <sheet name="Web_Page_Test_Desktop" r:id="rId2" sheetId="2"/>
+    <sheet name="Page_Speed_Insight" r:id="rId3" sheetId="3"/>
   </sheets>
   <calcPr calcId="144525"/>
   <oleSize ref="A1:C11"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="11">
   <si>
     <t>Urls</t>
   </si>
@@ -256,7 +256,79 @@
     <t>Desktop</t>
   </si>
   <si>
+    <t>45%</t>
+  </si>
+  <si>
+    <t>98%</t>
+  </si>
+  <si>
     <t/>
+  </si>
+  <si>
+    <t>86%</t>
+  </si>
+  <si>
+    <t>91%</t>
+  </si>
+  <si>
+    <t>78%</t>
+  </si>
+  <si>
+    <t>18%</t>
+  </si>
+  <si>
+    <t>73%</t>
+  </si>
+  <si>
+    <t>14%</t>
+  </si>
+  <si>
+    <t>65%</t>
+  </si>
+  <si>
+    <t>92%</t>
+  </si>
+  <si>
+    <t>99%</t>
+  </si>
+  <si>
+    <t>33%</t>
+  </si>
+  <si>
+    <t>87%</t>
+  </si>
+  <si>
+    <t>40%</t>
+  </si>
+  <si>
+    <t>96%</t>
+  </si>
+  <si>
+    <t>85%</t>
+  </si>
+  <si>
+    <t>100%</t>
+  </si>
+  <si>
+    <t>50%</t>
+  </si>
+  <si>
+    <t>19%</t>
+  </si>
+  <si>
+    <t>15%</t>
+  </si>
+  <si>
+    <t>68%</t>
+  </si>
+  <si>
+    <t>95%</t>
+  </si>
+  <si>
+    <t>38%</t>
+  </si>
+  <si>
+    <t>94%</t>
   </si>
 </sst>
 </file>
@@ -264,12 +336,12 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ &quot;₹&quot;\ * #,##0_ ;_ &quot;₹&quot;\ * \-#,##0_ ;_ &quot;₹&quot;\ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="_ &quot;₹&quot;\ * #,##0.00_ ;_ &quot;₹&quot;\ * \-#,##0.00_ ;_ &quot;₹&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="179" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_ &quot;₹&quot;\ * #,##0_ ;_ &quot;₹&quot;\ * \-#,##0_ ;_ &quot;₹&quot;\ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;\ * #,##0.00_ ;_ &quot;₹&quot;\ * \-#,##0.00_ ;_ &quot;₹&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="23">
+  <fonts count="22">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -284,12 +356,6 @@
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <charset val="134"/>
     </font>
     <font>
       <sz val="10"/>
@@ -299,7 +365,15 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -314,10 +388,17 @@
     </font>
     <font>
       <b/>
-      <sz val="18"/>
+      <sz val="15"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -329,8 +410,24 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -343,15 +440,17 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -359,21 +458,14 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -387,40 +479,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -434,11 +494,17 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -463,187 +529,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -685,30 +751,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -742,17 +784,23 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -764,6 +812,15 @@
       </top>
       <bottom style="double">
         <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -782,234 +839,243 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="11" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="23" fontId="7" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="0" numFmtId="176">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="0" numFmtId="177">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="0" numFmtId="178">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="0" numFmtId="179">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="0" numFmtId="9">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyNumberFormat="0" applyProtection="0" borderId="6" fillId="13" fontId="8" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="5" fillId="0" fontId="5" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyFont="0" applyNumberFormat="0" applyProtection="0" borderId="4" fillId="8" fontId="0" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="14" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="22" fontId="3" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="10" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="12" fontId="7" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="16" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="20" fontId="7" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="13" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="17" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="5" fillId="0" fontId="6" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="8" fillId="0" fontId="15" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="15" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyNumberFormat="0" applyProtection="0" borderId="3" fillId="19" fontId="12" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="11" fontId="3" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="31" fontId="20" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyNumberFormat="0" applyProtection="0" borderId="9" fillId="7" fontId="19" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="30" fontId="7" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyNumberFormat="0" applyProtection="0" borderId="3" fillId="7" fontId="4" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="10" fillId="0" fontId="21" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="7" fillId="0" fontId="9" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="29" fontId="18" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="18" fontId="11" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="26" fontId="3" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="34" fontId="7" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="6" fontId="3" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="5" fontId="3" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="25" fontId="7" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="16" fontId="7" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="15" fontId="3" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="4" fontId="3" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="28" fontId="7" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="14" fontId="3" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="33" fontId="7" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="21" fontId="7" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="10" fontId="3" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="17" fontId="7" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="32" fontId="3" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="24" fontId="3" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="27" fontId="7" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="9" fontId="3" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
   <cellXfs count="8">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="1" fillId="2" fontId="1" numFmtId="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyBorder="1" borderId="2" fillId="0" fontId="0" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" borderId="2" fillId="0" fontId="0" numFmtId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="2" fillId="0" fontId="2" numFmtId="9" xfId="0">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="9" fontId="3" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="2" fillId="3" fontId="2" numFmtId="9" xfId="0">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" borderId="2" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="2" fillId="2" fontId="1" numFmtId="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="40% - Accent1" xfId="1" builtinId="31"/>
-    <cellStyle name="Comma" xfId="2" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="3" builtinId="6"/>
-    <cellStyle name="Currency [0]" xfId="4" builtinId="7"/>
-    <cellStyle name="Currency" xfId="5" builtinId="4"/>
-    <cellStyle name="Percent" xfId="6" builtinId="5"/>
-    <cellStyle name="Check Cell" xfId="7" builtinId="23"/>
-    <cellStyle name="Heading 2" xfId="8" builtinId="17"/>
-    <cellStyle name="Note" xfId="9" builtinId="10"/>
-    <cellStyle name="Hyperlink" xfId="10" builtinId="8"/>
-    <cellStyle name="60% - Accent4" xfId="11" builtinId="44"/>
-    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9"/>
-    <cellStyle name="40% - Accent3" xfId="13" builtinId="39"/>
-    <cellStyle name="Warning Text" xfId="14" builtinId="11"/>
-    <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
-    <cellStyle name="Title" xfId="16" builtinId="15"/>
-    <cellStyle name="CExplanatory Text" xfId="17" builtinId="53"/>
-    <cellStyle name="Heading 1" xfId="18" builtinId="16"/>
-    <cellStyle name="Heading 3" xfId="19" builtinId="18"/>
-    <cellStyle name="Heading 4" xfId="20" builtinId="19"/>
-    <cellStyle name="Input" xfId="21" builtinId="20"/>
-    <cellStyle name="60% - Accent3" xfId="22" builtinId="40"/>
-    <cellStyle name="Good" xfId="23" builtinId="26"/>
-    <cellStyle name="Output" xfId="24" builtinId="21"/>
-    <cellStyle name="20% - Accent1" xfId="25" builtinId="30"/>
-    <cellStyle name="Calculation" xfId="26" builtinId="22"/>
-    <cellStyle name="Linked Cell" xfId="27" builtinId="24"/>
-    <cellStyle name="Total" xfId="28" builtinId="25"/>
-    <cellStyle name="Bad" xfId="29" builtinId="27"/>
-    <cellStyle name="Neutral" xfId="30" builtinId="28"/>
-    <cellStyle name="Accent1" xfId="31" builtinId="29"/>
-    <cellStyle name="20% - Accent5" xfId="32" builtinId="46"/>
-    <cellStyle name="60% - Accent1" xfId="33" builtinId="32"/>
-    <cellStyle name="Accent2" xfId="34" builtinId="33"/>
-    <cellStyle name="20% - Accent2" xfId="35" builtinId="34"/>
-    <cellStyle name="20% - Accent6" xfId="36" builtinId="50"/>
-    <cellStyle name="60% - Accent2" xfId="37" builtinId="36"/>
-    <cellStyle name="Accent3" xfId="38" builtinId="37"/>
-    <cellStyle name="20% - Accent3" xfId="39" builtinId="38"/>
-    <cellStyle name="Accent4" xfId="40" builtinId="41"/>
-    <cellStyle name="20% - Accent4" xfId="41" builtinId="42"/>
-    <cellStyle name="40% - Accent4" xfId="42" builtinId="43"/>
-    <cellStyle name="Accent5" xfId="43" builtinId="45"/>
-    <cellStyle name="40% - Accent5" xfId="44" builtinId="47"/>
-    <cellStyle name="60% - Accent5" xfId="45" builtinId="48"/>
-    <cellStyle name="Accent6" xfId="46" builtinId="49"/>
-    <cellStyle name="40% - Accent6" xfId="47" builtinId="51"/>
-    <cellStyle name="60% - Accent6" xfId="48" builtinId="52"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle builtinId="31" name="40% - Accent1" xfId="1"/>
+    <cellStyle builtinId="3" name="Comma" xfId="2"/>
+    <cellStyle builtinId="6" name="Comma [0]" xfId="3"/>
+    <cellStyle builtinId="7" name="Currency [0]" xfId="4"/>
+    <cellStyle builtinId="4" name="Currency" xfId="5"/>
+    <cellStyle builtinId="5" name="Percent" xfId="6"/>
+    <cellStyle builtinId="23" name="Check Cell" xfId="7"/>
+    <cellStyle builtinId="17" name="Heading 2" xfId="8"/>
+    <cellStyle builtinId="10" name="Note" xfId="9"/>
+    <cellStyle builtinId="8" name="Hyperlink" xfId="10"/>
+    <cellStyle builtinId="44" name="60% - Accent4" xfId="11"/>
+    <cellStyle builtinId="9" name="Followed Hyperlink" xfId="12"/>
+    <cellStyle builtinId="39" name="40% - Accent3" xfId="13"/>
+    <cellStyle builtinId="11" name="Warning Text" xfId="14"/>
+    <cellStyle builtinId="35" name="40% - Accent2" xfId="15"/>
+    <cellStyle builtinId="15" name="Title" xfId="16"/>
+    <cellStyle builtinId="53" name="CExplanatory Text" xfId="17"/>
+    <cellStyle builtinId="16" name="Heading 1" xfId="18"/>
+    <cellStyle builtinId="18" name="Heading 3" xfId="19"/>
+    <cellStyle builtinId="19" name="Heading 4" xfId="20"/>
+    <cellStyle builtinId="20" name="Input" xfId="21"/>
+    <cellStyle builtinId="40" name="60% - Accent3" xfId="22"/>
+    <cellStyle builtinId="26" name="Good" xfId="23"/>
+    <cellStyle builtinId="21" name="Output" xfId="24"/>
+    <cellStyle builtinId="30" name="20% - Accent1" xfId="25"/>
+    <cellStyle builtinId="22" name="Calculation" xfId="26"/>
+    <cellStyle builtinId="24" name="Linked Cell" xfId="27"/>
+    <cellStyle builtinId="25" name="Total" xfId="28"/>
+    <cellStyle builtinId="27" name="Bad" xfId="29"/>
+    <cellStyle builtinId="28" name="Neutral" xfId="30"/>
+    <cellStyle builtinId="29" name="Accent1" xfId="31"/>
+    <cellStyle builtinId="46" name="20% - Accent5" xfId="32"/>
+    <cellStyle builtinId="32" name="60% - Accent1" xfId="33"/>
+    <cellStyle builtinId="33" name="Accent2" xfId="34"/>
+    <cellStyle builtinId="34" name="20% - Accent2" xfId="35"/>
+    <cellStyle builtinId="50" name="20% - Accent6" xfId="36"/>
+    <cellStyle builtinId="36" name="60% - Accent2" xfId="37"/>
+    <cellStyle builtinId="37" name="Accent3" xfId="38"/>
+    <cellStyle builtinId="38" name="20% - Accent3" xfId="39"/>
+    <cellStyle builtinId="41" name="Accent4" xfId="40"/>
+    <cellStyle builtinId="42" name="20% - Accent4" xfId="41"/>
+    <cellStyle builtinId="43" name="40% - Accent4" xfId="42"/>
+    <cellStyle builtinId="45" name="Accent5" xfId="43"/>
+    <cellStyle builtinId="47" name="40% - Accent5" xfId="44"/>
+    <cellStyle builtinId="48" name="60% - Accent5" xfId="45"/>
+    <cellStyle builtinId="49" name="Accent6" xfId="46"/>
+    <cellStyle builtinId="51" name="40% - Accent6" xfId="47"/>
+    <cellStyle builtinId="52" name="60% - Accent6" xfId="48"/>
   </cellStyles>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -1023,10 +1089,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -1190,21 +1256,21 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="6350">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="12700">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="19050">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -1221,7 +1287,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw algn="ctr" blurRad="57150" dir="5400000" dist="19050" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -1274,9 +1340,9 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <sheetPr/>
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1284,12 +1350,12 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="2"/>
   <cols>
-    <col min="1" max="1" width="34.2857142857143" customWidth="1"/>
-    <col min="2" max="2" width="21.2857142857143" customWidth="1"/>
-    <col min="3" max="3" width="80.8571428571429" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="34.2857142857143" collapsed="false"/>
+    <col min="2" max="2" customWidth="true" width="21.2857142857143" collapsed="false"/>
+    <col min="3" max="3" customWidth="true" width="80.8571428571429" collapsed="false"/>
   </cols>
   <sheetData>
-    <row r="1" ht="30" spans="1:3">
+    <row ht="30" r="1" spans="1:3">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -1301,125 +1367,125 @@
       </c>
     </row>
     <row r="2" spans="1:3">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B2" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="2" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:3">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B3" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="2" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:3">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B4" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="2" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:3">
-      <c r="A5" s="3" t="s">
+      <c r="A5" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B5" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="2" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:3">
-      <c r="A6" s="3" t="s">
+      <c r="A6" s="2" t="s">
         <v>15</v>
       </c>
       <c r="B6" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="2" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="7" spans="1:3">
-      <c r="A7" s="3" t="s">
+      <c r="A7" s="2" t="s">
         <v>18</v>
       </c>
       <c r="B7" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="C7" s="2" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:3">
-      <c r="A8" s="3" t="s">
+      <c r="A8" s="2" t="s">
         <v>21</v>
       </c>
       <c r="B8" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="C8" s="2" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="9" spans="1:3">
-      <c r="A9" s="3" t="s">
+      <c r="A9" s="2" t="s">
         <v>24</v>
       </c>
       <c r="B9" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="C9" s="2" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="10" spans="1:3">
-      <c r="A10" s="3" t="s">
+      <c r="A10" s="2" t="s">
         <v>27</v>
       </c>
       <c r="B10" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="C10" s="2" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="11" spans="1:3">
-      <c r="A11" s="3" t="s">
+      <c r="A11" s="2" t="s">
         <v>30</v>
       </c>
       <c r="B11" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="C11" s="3" t="s">
+      <c r="C11" s="2" t="s">
         <v>32</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
+  <pageMargins bottom="1" footer="0.511805555555556" header="0.511805555555556" left="0.75" right="0.75" top="1"/>
   <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <sheetPr/>
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B18" sqref="B18"/>
@@ -1427,14 +1493,14 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="4"/>
   <cols>
-    <col min="1" max="1" width="37.5714285714286" customWidth="1"/>
-    <col min="2" max="2" width="9.85714285714286" customWidth="1"/>
-    <col min="3" max="3" width="8.85714285714286" customWidth="1"/>
-    <col min="4" max="4" width="14" customWidth="1"/>
-    <col min="5" max="5" width="89.2857142857143" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="37.5714285714286" collapsed="false"/>
+    <col min="2" max="2" customWidth="true" width="9.85714285714286" collapsed="false"/>
+    <col min="3" max="3" customWidth="true" width="8.85714285714286" collapsed="false"/>
+    <col min="4" max="4" customWidth="true" width="14.0" collapsed="false"/>
+    <col min="5" max="5" customWidth="true" width="89.2857142857143" collapsed="false"/>
   </cols>
   <sheetData>
-    <row r="1" ht="30" spans="1:5">
+    <row ht="30" r="1" spans="1:5">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -1452,7 +1518,7 @@
       </c>
     </row>
     <row r="2" spans="1:5">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B2" s="6" t="s">
@@ -1464,12 +1530,12 @@
       <c r="D2" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="2" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:5">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B3" s="6" t="s">
@@ -1481,12 +1547,12 @@
       <c r="D3" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="E3" s="2" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="4" spans="1:5">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B4" s="6" t="s">
@@ -1498,12 +1564,12 @@
       <c r="D4" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="E4" s="2" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="5" spans="1:5">
-      <c r="A5" s="3" t="s">
+      <c r="A5" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B5" s="6" t="s">
@@ -1515,12 +1581,12 @@
       <c r="D5" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="E5" s="3" t="s">
+      <c r="E5" s="2" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="6" spans="1:5">
-      <c r="A6" s="3" t="s">
+      <c r="A6" s="2" t="s">
         <v>15</v>
       </c>
       <c r="B6" s="6" t="s">
@@ -1532,12 +1598,12 @@
       <c r="D6" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="E6" s="3" t="s">
+      <c r="E6" s="2" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="7" spans="1:5">
-      <c r="A7" s="3" t="s">
+      <c r="A7" s="2" t="s">
         <v>18</v>
       </c>
       <c r="B7" s="6" t="s">
@@ -1549,12 +1615,12 @@
       <c r="D7" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="E7" s="3" t="s">
+      <c r="E7" s="2" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="8" spans="1:5">
-      <c r="A8" s="3" t="s">
+      <c r="A8" s="2" t="s">
         <v>21</v>
       </c>
       <c r="B8" s="6" t="s">
@@ -1566,12 +1632,12 @@
       <c r="D8" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="E8" s="3" t="s">
+      <c r="E8" s="2" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="9" spans="1:5">
-      <c r="A9" s="3" t="s">
+      <c r="A9" s="2" t="s">
         <v>24</v>
       </c>
       <c r="B9" s="6" t="s">
@@ -1583,12 +1649,12 @@
       <c r="D9" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="E9" s="3" t="s">
+      <c r="E9" s="2" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="10" spans="1:5">
-      <c r="A10" s="3" t="s">
+      <c r="A10" s="2" t="s">
         <v>27</v>
       </c>
       <c r="B10" s="6" t="s">
@@ -1600,12 +1666,12 @@
       <c r="D10" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="E10" s="3" t="s">
+      <c r="E10" s="2" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="11" spans="1:5">
-      <c r="A11" s="3" t="s">
+      <c r="A11" s="2" t="s">
         <v>30</v>
       </c>
       <c r="B11" s="6" t="s">
@@ -1617,99 +1683,127 @@
       <c r="D11" s="6" t="s">
         <v>75</v>
       </c>
-      <c r="E11" s="3" t="s">
+      <c r="E11" s="2" t="s">
         <v>76</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
+  <pageMargins bottom="1" footer="0.511805555555556" header="0.511805555555556" left="0.75" right="0.75" top="1"/>
   <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <sheetPr/>
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B2" sqref="B2:C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="7" outlineLevelCol="3"/>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="3" outlineLevelRow="7"/>
   <cols>
-    <col min="1" max="1" width="37.5714285714286" customWidth="1"/>
-    <col min="3" max="3" width="12.2857142857143" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="37.5714285714286" collapsed="false"/>
+    <col min="3" max="3" customWidth="true" width="12.2857142857143" collapsed="false"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="2" spans="1:4">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
+      <c r="B2" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>94</v>
+      </c>
       <c r="D2" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
     </row>
     <row r="3" spans="1:4">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="4"/>
-      <c r="C3" s="4"/>
+      <c r="B3" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>96</v>
+      </c>
       <c r="D3" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
     </row>
     <row r="4" spans="1:3">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="4"/>
-      <c r="C4" s="4"/>
+      <c r="B4" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>96</v>
+      </c>
     </row>
     <row r="5" spans="1:3">
-      <c r="A5" s="3" t="s">
+      <c r="A5" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B5" s="4"/>
-      <c r="C5" s="4"/>
+      <c r="B5" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="6" spans="1:3">
-      <c r="A6" s="3" t="s">
+      <c r="A6" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B6" s="5"/>
-      <c r="C6" s="4"/>
+      <c r="B6" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>100</v>
+      </c>
     </row>
     <row r="7" spans="1:3">
-      <c r="A7" s="3" t="s">
+      <c r="A7" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B7" s="6"/>
-      <c r="C7" s="6"/>
+      <c r="B7" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>96</v>
+      </c>
     </row>
     <row r="8" spans="1:3">
-      <c r="A8" s="3" t="s">
+      <c r="A8" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B8" s="6"/>
-      <c r="C8" s="6"/>
+      <c r="B8" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>103</v>
+      </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
+  <pageMargins bottom="1" footer="0.511805555555556" header="0.511805555555556" left="0.75" right="0.75" top="1"/>
   <headerFooter/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Performance file by manik on 16.11.2018.15.54
</commit_message>
<xml_diff>
--- a/data/Performance_Audit.xlsx
+++ b/data/Performance_Audit.xlsx
@@ -4,12 +4,12 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="14640" windowHeight="4305" activeTab="2"/>
+    <workbookView activeTab="2" windowHeight="4305" windowWidth="14640"/>
   </bookViews>
   <sheets>
-    <sheet name="Web_Page_Test_Mobile" sheetId="1" r:id="rId1"/>
-    <sheet name="Web_Page_Test_Desktop" sheetId="2" r:id="rId2"/>
-    <sheet name="Page_Insight" sheetId="3" r:id="rId3"/>
+    <sheet name="Web_Page_Test_Mobile" r:id="rId1" sheetId="1"/>
+    <sheet name="Web_Page_Test_Desktop" r:id="rId2" sheetId="2"/>
+    <sheet name="Page_Insight" r:id="rId3" sheetId="3"/>
   </sheets>
   <calcPr calcId="144525"/>
   <oleSize ref="A1:C11"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="7">
   <si>
     <t>Urls</t>
   </si>
@@ -257,6 +257,27 @@
   </si>
   <si>
     <t/>
+  </si>
+  <si>
+    <t>47</t>
+  </si>
+  <si>
+    <t>98</t>
+  </si>
+  <si>
+    <t>84</t>
+  </si>
+  <si>
+    <t>100</t>
+  </si>
+  <si>
+    <t>26</t>
+  </si>
+  <si>
+    <t>82</t>
+  </si>
+  <si>
+    <t>14</t>
   </si>
 </sst>
 </file>
@@ -784,232 +805,232 @@
     </border>
   </borders>
   <cellStyleXfs count="49">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="11" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="14" fontId="14" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="0" numFmtId="179">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="0" numFmtId="176">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="0" numFmtId="177">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="0" numFmtId="178">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="0" numFmtId="9">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyNumberFormat="0" applyProtection="0" borderId="4" fillId="5" fontId="7" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="3" fillId="0" fontId="5" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyFont="0" applyNumberFormat="0" applyProtection="0" borderId="6" fillId="9" fontId="0" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="16" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="19" fontId="10" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="19" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="13" fontId="14" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="13" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="21" fontId="14" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="6" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="15" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="3" fillId="0" fontId="22" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="8" fillId="0" fontId="18" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="18" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyNumberFormat="0" applyProtection="0" borderId="5" fillId="7" fontId="9" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="23" fontId="10" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="4" fontId="4" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyNumberFormat="0" applyProtection="0" borderId="10" fillId="11" fontId="21" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="18" fontId="14" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyNumberFormat="0" applyProtection="0" borderId="5" fillId="11" fontId="12" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="7" fillId="0" fontId="17" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="9" fillId="0" fontId="20" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="6" fontId="8" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="10" fontId="11" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="8" fontId="10" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="25" fontId="14" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="20" fontId="10" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="27" fontId="10" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="24" fontId="14" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="32" fontId="14" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="31" fontId="10" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="22" fontId="10" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="17" fontId="14" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="34" fontId="10" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="30" fontId="14" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="33" fontId="14" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="12" fontId="10" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="29" fontId="14" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="16" fontId="10" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="26" fontId="10" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="28" fontId="14" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="15" fontId="10" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
   <cellXfs count="8">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="1" fillId="2" fontId="1" numFmtId="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="2" fillId="3" fontId="2" numFmtId="0" xfId="0">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyBorder="1" borderId="2" fillId="0" fontId="0" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="2" fillId="0" fontId="3" numFmtId="9" xfId="0">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="9" fontId="3" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="2" fillId="3" fontId="3" numFmtId="9" xfId="0">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" borderId="2" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="2" fillId="2" fontId="1" numFmtId="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="40% - Accent1" xfId="1" builtinId="31"/>
-    <cellStyle name="Comma" xfId="2" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="3" builtinId="6"/>
-    <cellStyle name="Currency [0]" xfId="4" builtinId="7"/>
-    <cellStyle name="Currency" xfId="5" builtinId="4"/>
-    <cellStyle name="Percent" xfId="6" builtinId="5"/>
-    <cellStyle name="Check Cell" xfId="7" builtinId="23"/>
-    <cellStyle name="Heading 2" xfId="8" builtinId="17"/>
-    <cellStyle name="Note" xfId="9" builtinId="10"/>
-    <cellStyle name="Hyperlink" xfId="10" builtinId="8"/>
-    <cellStyle name="60% - Accent4" xfId="11" builtinId="44"/>
-    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9"/>
-    <cellStyle name="40% - Accent3" xfId="13" builtinId="39"/>
-    <cellStyle name="Warning Text" xfId="14" builtinId="11"/>
-    <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
-    <cellStyle name="Title" xfId="16" builtinId="15"/>
-    <cellStyle name="CExplanatory Text" xfId="17" builtinId="53"/>
-    <cellStyle name="Heading 1" xfId="18" builtinId="16"/>
-    <cellStyle name="Heading 3" xfId="19" builtinId="18"/>
-    <cellStyle name="Heading 4" xfId="20" builtinId="19"/>
-    <cellStyle name="Input" xfId="21" builtinId="20"/>
-    <cellStyle name="60% - Accent3" xfId="22" builtinId="40"/>
-    <cellStyle name="Good" xfId="23" builtinId="26"/>
-    <cellStyle name="Output" xfId="24" builtinId="21"/>
-    <cellStyle name="20% - Accent1" xfId="25" builtinId="30"/>
-    <cellStyle name="Calculation" xfId="26" builtinId="22"/>
-    <cellStyle name="Linked Cell" xfId="27" builtinId="24"/>
-    <cellStyle name="Total" xfId="28" builtinId="25"/>
-    <cellStyle name="Bad" xfId="29" builtinId="27"/>
-    <cellStyle name="Neutral" xfId="30" builtinId="28"/>
-    <cellStyle name="Accent1" xfId="31" builtinId="29"/>
-    <cellStyle name="20% - Accent5" xfId="32" builtinId="46"/>
-    <cellStyle name="60% - Accent1" xfId="33" builtinId="32"/>
-    <cellStyle name="Accent2" xfId="34" builtinId="33"/>
-    <cellStyle name="20% - Accent2" xfId="35" builtinId="34"/>
-    <cellStyle name="20% - Accent6" xfId="36" builtinId="50"/>
-    <cellStyle name="60% - Accent2" xfId="37" builtinId="36"/>
-    <cellStyle name="Accent3" xfId="38" builtinId="37"/>
-    <cellStyle name="20% - Accent3" xfId="39" builtinId="38"/>
-    <cellStyle name="Accent4" xfId="40" builtinId="41"/>
-    <cellStyle name="20% - Accent4" xfId="41" builtinId="42"/>
-    <cellStyle name="40% - Accent4" xfId="42" builtinId="43"/>
-    <cellStyle name="Accent5" xfId="43" builtinId="45"/>
-    <cellStyle name="40% - Accent5" xfId="44" builtinId="47"/>
-    <cellStyle name="60% - Accent5" xfId="45" builtinId="48"/>
-    <cellStyle name="Accent6" xfId="46" builtinId="49"/>
-    <cellStyle name="40% - Accent6" xfId="47" builtinId="51"/>
-    <cellStyle name="60% - Accent6" xfId="48" builtinId="52"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle builtinId="31" name="40% - Accent1" xfId="1"/>
+    <cellStyle builtinId="3" name="Comma" xfId="2"/>
+    <cellStyle builtinId="6" name="Comma [0]" xfId="3"/>
+    <cellStyle builtinId="7" name="Currency [0]" xfId="4"/>
+    <cellStyle builtinId="4" name="Currency" xfId="5"/>
+    <cellStyle builtinId="5" name="Percent" xfId="6"/>
+    <cellStyle builtinId="23" name="Check Cell" xfId="7"/>
+    <cellStyle builtinId="17" name="Heading 2" xfId="8"/>
+    <cellStyle builtinId="10" name="Note" xfId="9"/>
+    <cellStyle builtinId="8" name="Hyperlink" xfId="10"/>
+    <cellStyle builtinId="44" name="60% - Accent4" xfId="11"/>
+    <cellStyle builtinId="9" name="Followed Hyperlink" xfId="12"/>
+    <cellStyle builtinId="39" name="40% - Accent3" xfId="13"/>
+    <cellStyle builtinId="11" name="Warning Text" xfId="14"/>
+    <cellStyle builtinId="35" name="40% - Accent2" xfId="15"/>
+    <cellStyle builtinId="15" name="Title" xfId="16"/>
+    <cellStyle builtinId="53" name="CExplanatory Text" xfId="17"/>
+    <cellStyle builtinId="16" name="Heading 1" xfId="18"/>
+    <cellStyle builtinId="18" name="Heading 3" xfId="19"/>
+    <cellStyle builtinId="19" name="Heading 4" xfId="20"/>
+    <cellStyle builtinId="20" name="Input" xfId="21"/>
+    <cellStyle builtinId="40" name="60% - Accent3" xfId="22"/>
+    <cellStyle builtinId="26" name="Good" xfId="23"/>
+    <cellStyle builtinId="21" name="Output" xfId="24"/>
+    <cellStyle builtinId="30" name="20% - Accent1" xfId="25"/>
+    <cellStyle builtinId="22" name="Calculation" xfId="26"/>
+    <cellStyle builtinId="24" name="Linked Cell" xfId="27"/>
+    <cellStyle builtinId="25" name="Total" xfId="28"/>
+    <cellStyle builtinId="27" name="Bad" xfId="29"/>
+    <cellStyle builtinId="28" name="Neutral" xfId="30"/>
+    <cellStyle builtinId="29" name="Accent1" xfId="31"/>
+    <cellStyle builtinId="46" name="20% - Accent5" xfId="32"/>
+    <cellStyle builtinId="32" name="60% - Accent1" xfId="33"/>
+    <cellStyle builtinId="33" name="Accent2" xfId="34"/>
+    <cellStyle builtinId="34" name="20% - Accent2" xfId="35"/>
+    <cellStyle builtinId="50" name="20% - Accent6" xfId="36"/>
+    <cellStyle builtinId="36" name="60% - Accent2" xfId="37"/>
+    <cellStyle builtinId="37" name="Accent3" xfId="38"/>
+    <cellStyle builtinId="38" name="20% - Accent3" xfId="39"/>
+    <cellStyle builtinId="41" name="Accent4" xfId="40"/>
+    <cellStyle builtinId="42" name="20% - Accent4" xfId="41"/>
+    <cellStyle builtinId="43" name="40% - Accent4" xfId="42"/>
+    <cellStyle builtinId="45" name="Accent5" xfId="43"/>
+    <cellStyle builtinId="47" name="40% - Accent5" xfId="44"/>
+    <cellStyle builtinId="48" name="60% - Accent5" xfId="45"/>
+    <cellStyle builtinId="49" name="Accent6" xfId="46"/>
+    <cellStyle builtinId="51" name="40% - Accent6" xfId="47"/>
+    <cellStyle builtinId="52" name="60% - Accent6" xfId="48"/>
   </cellStyles>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -1023,10 +1044,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -1190,21 +1211,21 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="6350">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="12700">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="19050">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -1221,7 +1242,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw algn="ctr" blurRad="57150" dir="5400000" dist="19050" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -1274,9 +1295,9 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <sheetPr/>
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1284,12 +1305,12 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="2"/>
   <cols>
-    <col min="1" max="1" width="34.2857142857143" customWidth="1"/>
-    <col min="2" max="2" width="21.2857142857143" customWidth="1"/>
-    <col min="3" max="3" width="80.8571428571429" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="34.2857142857143" collapsed="false"/>
+    <col min="2" max="2" customWidth="true" width="21.2857142857143" collapsed="false"/>
+    <col min="3" max="3" customWidth="true" width="80.8571428571429" collapsed="false"/>
   </cols>
   <sheetData>
-    <row r="1" ht="30" spans="1:3">
+    <row ht="30" r="1" spans="1:3">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -1411,15 +1432,15 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
+  <pageMargins bottom="1" footer="0.511805555555556" header="0.511805555555556" left="0.75" right="0.75" top="1"/>
   <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <sheetPr/>
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B18" sqref="B18"/>
@@ -1427,14 +1448,14 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="4"/>
   <cols>
-    <col min="1" max="1" width="37.5714285714286" customWidth="1"/>
-    <col min="2" max="2" width="9.85714285714286" customWidth="1"/>
-    <col min="3" max="3" width="8.85714285714286" customWidth="1"/>
-    <col min="4" max="4" width="14" customWidth="1"/>
-    <col min="5" max="5" width="89.2857142857143" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="37.5714285714286" collapsed="false"/>
+    <col min="2" max="2" customWidth="true" width="9.85714285714286" collapsed="false"/>
+    <col min="3" max="3" customWidth="true" width="8.85714285714286" collapsed="false"/>
+    <col min="4" max="4" customWidth="true" width="14.0" collapsed="false"/>
+    <col min="5" max="5" customWidth="true" width="89.2857142857143" collapsed="false"/>
   </cols>
   <sheetData>
-    <row r="1" ht="30" spans="1:5">
+    <row ht="30" r="1" spans="1:5">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -1622,24 +1643,24 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
+  <pageMargins bottom="1" footer="0.511805555555556" header="0.511805555555556" left="0.75" right="0.75" top="1"/>
   <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <sheetPr/>
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B2" sqref="B2:C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="7" outlineLevelCol="3"/>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="3" outlineLevelRow="7"/>
   <cols>
-    <col min="1" max="1" width="37.5714285714286" customWidth="1"/>
-    <col min="3" max="3" width="12.2857142857143" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="37.5714285714286" collapsed="false"/>
+    <col min="3" max="3" customWidth="true" width="12.2857142857143" collapsed="false"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -1657,8 +1678,12 @@
       <c r="A2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
+      <c r="B2" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>81</v>
+      </c>
       <c r="D2" t="s">
         <v>79</v>
       </c>
@@ -1667,8 +1692,12 @@
       <c r="A3" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="4"/>
-      <c r="C3" s="4"/>
+      <c r="B3" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>83</v>
+      </c>
       <c r="D3" t="s">
         <v>79</v>
       </c>
@@ -1677,22 +1706,34 @@
       <c r="A4" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="4"/>
-      <c r="C4" s="4"/>
+      <c r="B4" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B5" s="4"/>
-      <c r="C5" s="4"/>
+      <c r="B5" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>85</v>
+      </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B6" s="5"/>
-      <c r="C6" s="4"/>
+      <c r="B6" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="3" t="s">
@@ -1709,7 +1750,7 @@
       <c r="C8" s="6"/>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
+  <pageMargins bottom="1" footer="0.511805555555556" header="0.511805555555556" left="0.75" right="0.75" top="1"/>
   <headerFooter/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Page count files updated by Manika prabu on 05.12.2018.14.56
</commit_message>
<xml_diff>
--- a/data/Performance_Audit.xlsx
+++ b/data/Performance_Audit.xlsx
@@ -4,12 +4,13 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="20385" windowHeight="8370"/>
+    <workbookView windowWidth="20295" windowHeight="7920" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Web_Page_Test_Mobile" sheetId="1" r:id="rId1"/>
     <sheet name="Web_Page_Test_Desktop" sheetId="2" r:id="rId2"/>
     <sheet name="Page_Insight" sheetId="3" r:id="rId3"/>
+    <sheet name="Site_Link" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="144525"/>
   <oleSize ref="A1:C11"/>
@@ -17,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21">
   <si>
     <t>Urls</t>
   </si>
@@ -77,6 +78,9 @@
   </si>
   <si>
     <t/>
+  </si>
+  <si>
+    <t>Page count</t>
   </si>
 </sst>
 </file>
@@ -84,9 +88,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ &quot;₹&quot;\ * #,##0_ ;_ &quot;₹&quot;\ * \-#,##0_ ;_ &quot;₹&quot;\ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ &quot;₹&quot;\ * #,##0.00_ ;_ &quot;₹&quot;\ * \-#,##0.00_ ;_ &quot;₹&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ &quot;₹&quot;\ * #,##0.00_ ;_ &quot;₹&quot;\ * \-#,##0.00_ ;_ &quot;₹&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_ &quot;₹&quot;\ * #,##0_ ;_ &quot;₹&quot;\ * \-#,##0_ ;_ &quot;₹&quot;\ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="179" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="22">
@@ -119,6 +123,98 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="18"/>
       <color theme="3"/>
@@ -127,130 +223,38 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="0"/>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -277,187 +281,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -480,7 +484,9 @@
       <top style="thin">
         <color auto="1"/>
       </top>
-      <bottom/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -493,8 +499,32 @@
       <top style="thin">
         <color auto="1"/>
       </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
       <bottom style="thin">
-        <color auto="1"/>
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -504,6 +534,21 @@
       <top/>
       <bottom style="medium">
         <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -519,17 +564,6 @@
       </top>
       <bottom style="double">
         <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -566,210 +600,177 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="25" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="6" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="23" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="26" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="20" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="20" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="2" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
@@ -1092,7 +1093,7 @@
   <sheetPr/>
   <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -1104,13 +1105,13 @@
   </cols>
   <sheetData>
     <row r="1" ht="30" spans="1:3">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
     </row>
@@ -1118,70 +1119,70 @@
       <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="6"/>
+      <c r="B2" s="3"/>
       <c r="C2" s="2"/>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="6"/>
+      <c r="B3" s="3"/>
       <c r="C3" s="2"/>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="6"/>
+      <c r="B4" s="3"/>
       <c r="C4" s="2"/>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="6"/>
+      <c r="B5" s="3"/>
       <c r="C5" s="2"/>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="6"/>
+      <c r="B6" s="3"/>
       <c r="C6" s="2"/>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="6"/>
+      <c r="B7" s="3"/>
       <c r="C7" s="2"/>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="6"/>
+      <c r="B8" s="3"/>
       <c r="C8" s="2"/>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="6"/>
+      <c r="B9" s="3"/>
       <c r="C9" s="2"/>
     </row>
     <row r="10" spans="1:3">
       <c r="A10" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B10" s="6"/>
+      <c r="B10" s="3"/>
       <c r="C10" s="2"/>
     </row>
     <row r="11" spans="1:3">
       <c r="A11" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B11" s="6"/>
+      <c r="B11" s="3"/>
       <c r="C11" s="2"/>
     </row>
   </sheetData>
@@ -1209,19 +1210,19 @@
   </cols>
   <sheetData>
     <row r="1" ht="30" spans="1:5">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="E1" s="1" t="s">
         <v>16</v>
       </c>
     </row>
@@ -1229,90 +1230,90 @@
       <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="6"/>
-      <c r="C2" s="6"/>
-      <c r="D2" s="6"/>
+      <c r="B2" s="3"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
       <c r="E2" s="2"/>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="6"/>
-      <c r="C3" s="6"/>
-      <c r="D3" s="6"/>
+      <c r="B3" s="3"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
       <c r="E3" s="2"/>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="6"/>
-      <c r="C4" s="6"/>
-      <c r="D4" s="6"/>
+      <c r="B4" s="3"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
       <c r="E4" s="2"/>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="6"/>
-      <c r="C5" s="6"/>
-      <c r="D5" s="6"/>
+      <c r="B5" s="3"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
       <c r="E5" s="2"/>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="6"/>
-      <c r="C6" s="6"/>
-      <c r="D6" s="6"/>
+      <c r="B6" s="3"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
       <c r="E6" s="2"/>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="6"/>
-      <c r="C7" s="6"/>
-      <c r="D7" s="6"/>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
       <c r="E7" s="2"/>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="6"/>
-      <c r="C8" s="6"/>
-      <c r="D8" s="6"/>
+      <c r="B8" s="3"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
       <c r="E8" s="2"/>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="6"/>
-      <c r="C9" s="6"/>
-      <c r="D9" s="6"/>
+      <c r="B9" s="3"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
       <c r="E9" s="2"/>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B10" s="6"/>
-      <c r="C10" s="6"/>
-      <c r="D10" s="6"/>
+      <c r="B10" s="3"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
       <c r="E10" s="2"/>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B11" s="6"/>
-      <c r="C11" s="6"/>
-      <c r="D11" s="6"/>
+      <c r="B11" s="3"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
       <c r="E11" s="2"/>
     </row>
   </sheetData>
@@ -1337,13 +1338,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="4" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1361,8 +1362,8 @@
       <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="4"/>
-      <c r="C3" s="4"/>
+      <c r="B3" s="5"/>
+      <c r="C3" s="5"/>
       <c r="D3" t="s">
         <v>19</v>
       </c>
@@ -1371,36 +1372,125 @@
       <c r="A4" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="4"/>
-      <c r="C4" s="4"/>
+      <c r="B4" s="5"/>
+      <c r="C4" s="5"/>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="4"/>
-      <c r="C5" s="4"/>
+      <c r="B5" s="5"/>
+      <c r="C5" s="5"/>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="5"/>
-      <c r="C6" s="4"/>
+      <c r="B6" s="6"/>
+      <c r="C6" s="5"/>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="6"/>
-      <c r="C7" s="6"/>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B8" s="6"/>
-      <c r="C8" s="6"/>
+      <c r="B8" s="3"/>
+      <c r="C8" s="3"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:B11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="1"/>
+  <cols>
+    <col min="1" max="1" width="37.5714285714286" customWidth="1"/>
+    <col min="2" max="2" width="13.2857142857143" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="3"/>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="3"/>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="3"/>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="3"/>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="3"/>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" s="3"/>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" s="3"/>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" s="3"/>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" s="3"/>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>

</xml_diff>

<commit_message>
Committed on 06:12:2018:13:20:00PM By Karthikeyan Rajendran
</commit_message>
<xml_diff>
--- a/data/Performance_Audit.xlsx
+++ b/data/Performance_Audit.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView activeTab="1" windowHeight="8370" windowWidth="20385"/>
+    <workbookView windowHeight="8370" windowWidth="20385"/>
   </bookViews>
   <sheets>
     <sheet name="Web_Page_Test_Mobile" r:id="rId1" sheetId="1"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="18">
   <si>
     <t>Urls</t>
   </si>
@@ -71,6 +71,126 @@
     <t>Desktop Result</t>
   </si>
   <si>
+    <t>3,519 KB</t>
+  </si>
+  <si>
+    <t>110</t>
+  </si>
+  <si>
+    <t>6.66</t>
+  </si>
+  <si>
+    <t>https://www.webpagetest.org/result/181205_7M_b0c6edbd36423d7dc17d9a44b3f821b7/</t>
+  </si>
+  <si>
+    <t>606 KB</t>
+  </si>
+  <si>
+    <t>25</t>
+  </si>
+  <si>
+    <t>1.94</t>
+  </si>
+  <si>
+    <t>https://www.webpagetest.org/result/181205_HF_68f1e6da3c96ff5bd196451011523983/</t>
+  </si>
+  <si>
+    <t>3,022 KB</t>
+  </si>
+  <si>
+    <t>64</t>
+  </si>
+  <si>
+    <t>6.16</t>
+  </si>
+  <si>
+    <t>https://www.webpagetest.org/result/181205_46_24eff7192d8eef52175acf7b7ed5d28d/</t>
+  </si>
+  <si>
+    <t>4,607 KB</t>
+  </si>
+  <si>
+    <t>87</t>
+  </si>
+  <si>
+    <t>9.99</t>
+  </si>
+  <si>
+    <t>https://www.webpagetest.org/result/181205_CE_565f78a1e473579040696ed1461a1e93/</t>
+  </si>
+  <si>
+    <t>15,686 KB</t>
+  </si>
+  <si>
+    <t>204</t>
+  </si>
+  <si>
+    <t>28.44</t>
+  </si>
+  <si>
+    <t>https://www.webpagetest.org/result/181205_SW_b3fae112090d8ecbd6a91c88129041e4/</t>
+  </si>
+  <si>
+    <t>3,423 KB</t>
+  </si>
+  <si>
+    <t>158</t>
+  </si>
+  <si>
+    <t>10.18</t>
+  </si>
+  <si>
+    <t>https://www.webpagetest.org/result/181205_KT_5b4243a5218918fbdda33519ea044b23/</t>
+  </si>
+  <si>
+    <t>826 KB</t>
+  </si>
+  <si>
+    <t>83</t>
+  </si>
+  <si>
+    <t>2.64</t>
+  </si>
+  <si>
+    <t>https://www.webpagetest.org/result/181205_RH_71c2932cbb44becff9ef0045ab02518d/</t>
+  </si>
+  <si>
+    <t>2,683 KB</t>
+  </si>
+  <si>
+    <t>42</t>
+  </si>
+  <si>
+    <t>4.91</t>
+  </si>
+  <si>
+    <t>https://www.webpagetest.org/result/181205_5P_064542f73e1a4704bd366b668597c0da/</t>
+  </si>
+  <si>
+    <t>3,531 KB</t>
+  </si>
+  <si>
+    <t>153</t>
+  </si>
+  <si>
+    <t>8.31</t>
+  </si>
+  <si>
+    <t>https://www.webpagetest.org/result/181205_89_38ee43094852377c9f06118f4107a349/</t>
+  </si>
+  <si>
+    <t>3,335 KB</t>
+  </si>
+  <si>
+    <t>80</t>
+  </si>
+  <si>
+    <t>6.88</t>
+  </si>
+  <si>
+    <t>https://www.webpagetest.org/result/181205_CT_b72b34eb5b8b547c063ff148bdbc3fd0/</t>
+  </si>
+  <si>
     <t>Mobile</t>
   </si>
   <si>
@@ -113,124 +233,58 @@
     <t>5,610</t>
   </si>
   <si>
-    <t>https://www.webpagetest.org/result/181205_7M_b0c6edbd36423d7dc17d9a44b3f821b7/</t>
-  </si>
-  <si>
-    <t>6.66</t>
-  </si>
-  <si>
-    <t>110</t>
-  </si>
-  <si>
-    <t>3,519 KB</t>
-  </si>
-  <si>
-    <t>https://www.webpagetest.org/result/181205_HF_68f1e6da3c96ff5bd196451011523983/</t>
-  </si>
-  <si>
-    <t>1.94</t>
-  </si>
-  <si>
-    <t>25</t>
-  </si>
-  <si>
-    <t>606 KB</t>
-  </si>
-  <si>
-    <t>https://www.webpagetest.org/result/181205_46_24eff7192d8eef52175acf7b7ed5d28d/</t>
-  </si>
-  <si>
-    <t>6.16</t>
-  </si>
-  <si>
-    <t>64</t>
-  </si>
-  <si>
-    <t>3,022 KB</t>
-  </si>
-  <si>
-    <t>https://www.webpagetest.org/result/181205_CE_565f78a1e473579040696ed1461a1e93/</t>
-  </si>
-  <si>
-    <t>9.99</t>
-  </si>
-  <si>
-    <t>87</t>
-  </si>
-  <si>
-    <t>4,607 KB</t>
-  </si>
-  <si>
-    <t>https://www.webpagetest.org/result/181205_SW_b3fae112090d8ecbd6a91c88129041e4/</t>
-  </si>
-  <si>
-    <t>28.44</t>
-  </si>
-  <si>
-    <t>204</t>
-  </si>
-  <si>
-    <t>15,686 KB</t>
-  </si>
-  <si>
-    <t>https://www.webpagetest.org/result/181205_KT_5b4243a5218918fbdda33519ea044b23/</t>
-  </si>
-  <si>
-    <t>10.18</t>
-  </si>
-  <si>
-    <t>158</t>
-  </si>
-  <si>
-    <t>3,423 KB</t>
-  </si>
-  <si>
-    <t>https://www.webpagetest.org/result/181205_RH_71c2932cbb44becff9ef0045ab02518d/</t>
-  </si>
-  <si>
-    <t>2.64</t>
-  </si>
-  <si>
-    <t>83</t>
-  </si>
-  <si>
-    <t>826 KB</t>
-  </si>
-  <si>
-    <t>https://www.webpagetest.org/result/181205_5P_064542f73e1a4704bd366b668597c0da/</t>
-  </si>
-  <si>
-    <t>4.91</t>
-  </si>
-  <si>
-    <t>42</t>
-  </si>
-  <si>
-    <t>2,683 KB</t>
-  </si>
-  <si>
-    <t>https://www.webpagetest.org/result/181205_89_38ee43094852377c9f06118f4107a349/</t>
-  </si>
-  <si>
-    <t>8.31</t>
-  </si>
-  <si>
-    <t>153</t>
-  </si>
-  <si>
-    <t>3,531 KB</t>
-  </si>
-  <si>
-    <t>https://www.webpagetest.org/result/181205_CT_b72b34eb5b8b547c063ff148bdbc3fd0/</t>
-  </si>
-  <si>
-    <t>6.88</t>
-  </si>
-  <si>
-    <t>80</t>
-  </si>
-  <si>
-    <t>3,335 KB</t>
+    <t>https://www.webpagetest.org/result/181206_4S_45876082867661b6b0310f16516e8c40/</t>
+  </si>
+  <si>
+    <t>3.61</t>
+  </si>
+  <si>
+    <t>https://www.webpagetest.org/result/181206_36_99d5ef8dcecd71e31ece19ae15e35f0e/</t>
+  </si>
+  <si>
+    <t>2.41</t>
+  </si>
+  <si>
+    <t>https://www.webpagetest.org/result/181206_QT_2edce564946c6d39455adfb8d8151274/</t>
+  </si>
+  <si>
+    <t>4.39</t>
+  </si>
+  <si>
+    <t>https://www.webpagetest.org/result/181206_K4_b9b1d866023ee222fd8d18bb8bc32dcc/</t>
+  </si>
+  <si>
+    <t>4.72</t>
+  </si>
+  <si>
+    <t>https://www.webpagetest.org/result/181206_TE_fa85411fde4cd0121b7e684295a21ade/</t>
+  </si>
+  <si>
+    <t>13.27</t>
+  </si>
+  <si>
+    <t>https://www.webpagetest.org/result/181206_E5_04bb12a04cb0c5b8be061b982c9d4cfa/</t>
+  </si>
+  <si>
+    <t>8.02</t>
+  </si>
+  <si>
+    <t>https://www.webpagetest.org/result/181206_Y3_8d13be0a6473aeb799c56eb23b44ceaf/</t>
+  </si>
+  <si>
+    <t>3.44</t>
+  </si>
+  <si>
+    <t>https://www.webpagetest.org/result/181206_4R_d9da7be055a3a165ef923bcb84a18fa4/</t>
+  </si>
+  <si>
+    <t>2.58</t>
+  </si>
+  <si>
+    <t>https://www.webpagetest.org/result/181206_71_9ab5b0dc16dfe2ea8340647bd3e013cd/</t>
+  </si>
+  <si>
+    <t>4.86</t>
   </si>
 </sst>
 </file>
@@ -238,10 +292,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ &quot;₹&quot;\ * #,##0_ ;_ &quot;₹&quot;\ * \-#,##0_ ;_ &quot;₹&quot;\ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;\ * #,##0.00_ ;_ &quot;₹&quot;\ * \-#,##0.00_ ;_ &quot;₹&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ &quot;₹&quot;\ * #,##0_ ;_ &quot;₹&quot;\ * \-#,##0_ ;_ &quot;₹&quot;\ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_ &quot;₹&quot;\ * #,##0.00_ ;_ &quot;₹&quot;\ * \-#,##0.00_ ;_ &quot;₹&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="22">
     <font>
@@ -274,7 +328,115 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -288,76 +450,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FF006100"/>
       <name val="Calibri"/>
@@ -365,44 +457,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
@@ -431,103 +485,169 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -539,73 +659,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -653,13 +707,32 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
       <top style="thin">
-        <color theme="4"/>
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
       </top>
       <bottom style="double">
-        <color theme="4"/>
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -669,6 +742,15 @@
       <top/>
       <bottom style="medium">
         <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -683,21 +765,6 @@
         <color rgb="FF3F3F3F"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
         <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
@@ -718,17 +785,13 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
+      <left/>
+      <right/>
       <top style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color theme="4"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -741,162 +804,153 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="24" fontId="8" numFmtId="0">
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="14" fontId="4" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="0" numFmtId="177">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="0" numFmtId="179">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="0" numFmtId="176">
       <alignment vertical="center"/>
     </xf>
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="0" numFmtId="178">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="0" numFmtId="176">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="0" numFmtId="177">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="0" numFmtId="179">
-      <alignment vertical="center"/>
-    </xf>
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="0" numFmtId="9">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="0" applyNumberFormat="0" applyProtection="0" borderId="6" fillId="11" fontId="12" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="4" fillId="0" fontId="7" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyFont="0" applyNumberFormat="0" applyProtection="0" borderId="8" fillId="19" fontId="0" numFmtId="0">
+    <xf applyAlignment="0" applyNumberFormat="0" applyProtection="0" borderId="4" fillId="8" fontId="5" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="5" fillId="0" fontId="6" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyFont="0" applyNumberFormat="0" applyProtection="0" borderId="3" fillId="7" fontId="0" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="12" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="21" fontId="3" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="8" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="26" fontId="4" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="15" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="18" fontId="4" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="11" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="16" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="5" fillId="0" fontId="14" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="10" fillId="0" fontId="10" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="10" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyNumberFormat="0" applyProtection="0" borderId="8" fillId="34" fontId="21" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="11" fontId="3" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="33" fontId="20" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyNumberFormat="0" applyProtection="0" borderId="7" fillId="17" fontId="13" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="20" fontId="4" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyNumberFormat="0" applyProtection="0" borderId="8" fillId="17" fontId="17" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="6" fillId="0" fontId="7" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="9" fillId="0" fontId="19" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="13" fontId="9" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="29" fontId="18" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="6" fontId="3" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="5" fontId="4" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="12" fontId="3" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="4" fontId="3" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="32" fontId="4" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="25" fontId="4" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="10" fontId="3" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="6" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="18" fontId="8" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="17" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="17" fontId="8" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="18" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="19" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="4" fillId="0" fontId="14" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="9" fillId="0" fontId="16" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="16" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyNumberFormat="0" applyProtection="0" borderId="7" fillId="34" fontId="21" numFmtId="0">
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="28" fontId="3" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="19" fontId="4" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="9" fontId="3" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="27" fontId="4" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="24" fontId="4" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="31" fontId="3" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="16" fontId="4" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="30" fontId="3" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
     <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="15" fontId="3" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="23" fontId="15" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyNumberFormat="0" applyProtection="0" borderId="5" fillId="9" fontId="10" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="33" fontId="8" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyNumberFormat="0" applyProtection="0" borderId="7" fillId="9" fontId="13" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="10" fillId="0" fontId="20" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="3" fillId="0" fontId="5" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="6" fontId="4" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="8" fontId="9" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="32" fontId="3" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="14" fontId="8" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="5" fontId="3" numFmtId="0">
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="23" fontId="4" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
     <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="22" fontId="3" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="21" fontId="8" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="30" fontId="8" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="13" fontId="3" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="27" fontId="3" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="7" fontId="8" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="26" fontId="3" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="16" fontId="8" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="29" fontId="8" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="25" fontId="3" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="31" fontId="8" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="4" fontId="3" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="28" fontId="3" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="12" fontId="8" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="20" fontId="3" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1243,8 +1297,8 @@
   <sheetPr/>
   <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="2"/>
@@ -1269,57 +1323,89 @@
       <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="3"/>
-      <c r="C2" s="2"/>
+      <c r="B2" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="3"/>
-      <c r="C3" s="2"/>
+      <c r="B3" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>73</v>
+      </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="3"/>
-      <c r="C4" s="2"/>
+      <c r="B4" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>75</v>
+      </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="3"/>
-      <c r="C5" s="2"/>
+      <c r="B5" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>77</v>
+      </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="3"/>
-      <c r="C6" s="2"/>
+      <c r="B6" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>79</v>
+      </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="3"/>
-      <c r="C7" s="2"/>
+      <c r="B7" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>81</v>
+      </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="3"/>
-      <c r="C8" s="2"/>
+      <c r="B8" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="3"/>
-      <c r="C9" s="2"/>
+      <c r="B9" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>85</v>
+      </c>
     </row>
     <row r="10" spans="1:3">
       <c r="A10" s="2" t="s">
@@ -1332,8 +1418,12 @@
       <c r="A11" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B11" s="3"/>
-      <c r="C11" s="2"/>
+      <c r="B11" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>87</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.511805555555556" header="0.511805555555556" left="0.75" right="0.75" top="1"/>
@@ -1346,7 +1436,7 @@
   <sheetPr/>
   <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -1381,16 +1471,16 @@
         <v>3</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>34</v>
+        <v>17</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>33</v>
+        <v>18</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>32</v>
+        <v>19</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -1398,16 +1488,16 @@
         <v>4</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>38</v>
+        <v>21</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>37</v>
+        <v>22</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>36</v>
+        <v>23</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -1415,16 +1505,16 @@
         <v>5</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>42</v>
+        <v>25</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>41</v>
+        <v>26</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>40</v>
+        <v>27</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>39</v>
+        <v>28</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -1432,16 +1522,16 @@
         <v>6</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>46</v>
+        <v>29</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>45</v>
+        <v>30</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>44</v>
+        <v>31</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>43</v>
+        <v>32</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -1449,16 +1539,16 @@
         <v>7</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>50</v>
+        <v>33</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>49</v>
+        <v>34</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>48</v>
+        <v>35</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -1466,16 +1556,16 @@
         <v>8</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>54</v>
+        <v>37</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>53</v>
+        <v>38</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>52</v>
+        <v>39</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>51</v>
+        <v>40</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -1483,16 +1573,16 @@
         <v>9</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>58</v>
+        <v>41</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>57</v>
+        <v>42</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>56</v>
+        <v>43</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>55</v>
+        <v>44</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -1500,16 +1590,16 @@
         <v>10</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>62</v>
+        <v>45</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>61</v>
+        <v>46</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>60</v>
+        <v>47</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -1517,16 +1607,16 @@
         <v>11</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>66</v>
+        <v>49</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>65</v>
+        <v>50</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>64</v>
+        <v>51</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>63</v>
+        <v>52</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -1534,16 +1624,16 @@
         <v>12</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>70</v>
+        <v>53</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>69</v>
+        <v>54</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>68</v>
+        <v>55</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>67</v>
+        <v>56</v>
       </c>
     </row>
   </sheetData>
@@ -1572,10 +1662,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>17</v>
+        <v>57</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>18</v>
+        <v>58</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -1585,7 +1675,7 @@
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
       <c r="D2" t="s">
-        <v>19</v>
+        <v>59</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -1595,7 +1685,7 @@
       <c r="B3" s="5"/>
       <c r="C3" s="5"/>
       <c r="D3" t="s">
-        <v>19</v>
+        <v>59</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -1659,7 +1749,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>20</v>
+        <v>60</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -1667,7 +1757,7 @@
         <v>3</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>21</v>
+        <v>61</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -1675,7 +1765,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>22</v>
+        <v>62</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -1683,7 +1773,7 @@
         <v>5</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>23</v>
+        <v>63</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -1691,7 +1781,7 @@
         <v>6</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>24</v>
+        <v>64</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -1699,7 +1789,7 @@
         <v>7</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>25</v>
+        <v>65</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -1707,7 +1797,7 @@
         <v>8</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>26</v>
+        <v>66</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -1715,7 +1805,7 @@
         <v>9</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>27</v>
+        <v>67</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -1723,7 +1813,7 @@
         <v>10</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>28</v>
+        <v>68</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -1731,7 +1821,7 @@
         <v>11</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>29</v>
+        <v>69</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -1739,7 +1829,7 @@
         <v>12</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>30</v>
+        <v>70</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Committed on 05:12:2018:22:00:02PM By Karthikeyan Rajendran
</commit_message>
<xml_diff>
--- a/data/Performance_Audit.xlsx
+++ b/data/Performance_Audit.xlsx
@@ -4,13 +4,13 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowHeight="8370" windowWidth="20385"/>
+    <workbookView windowWidth="20385" windowHeight="8370"/>
   </bookViews>
   <sheets>
-    <sheet name="Web_Page_Test_Mobile" r:id="rId1" sheetId="1"/>
-    <sheet name="Web_Page_Test_Desktop" r:id="rId2" sheetId="2"/>
-    <sheet name="Page_Insight" r:id="rId3" sheetId="3"/>
-    <sheet name="Page_Count" r:id="rId4" sheetId="4"/>
+    <sheet name="Web_Page_Test_Mobile" sheetId="1" r:id="rId1"/>
+    <sheet name="Web_Page_Test_Desktop" sheetId="2" r:id="rId2"/>
+    <sheet name="Page_Insight" sheetId="3" r:id="rId3"/>
+    <sheet name="Page_Count" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="144525"/>
   <oleSize ref="A1:C11"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91">
   <si>
     <t>Urls</t>
   </si>
@@ -32,33 +32,93 @@
     <t>https://www.sfwmd.gov/</t>
   </si>
   <si>
+    <t>3.61</t>
+  </si>
+  <si>
+    <t>https://www.webpagetest.org/result/181206_4S_45876082867661b6b0310f16516e8c40/</t>
+  </si>
+  <si>
     <t>https://www.nicb.org/</t>
   </si>
   <si>
+    <t>2.41</t>
+  </si>
+  <si>
+    <t>https://www.webpagetest.org/result/181206_36_99d5ef8dcecd71e31ece19ae15e35f0e/</t>
+  </si>
+  <si>
     <t>https://www.boston.gov/</t>
   </si>
   <si>
+    <t>4.39</t>
+  </si>
+  <si>
+    <t>https://www.webpagetest.org/result/181206_QT_2edce564946c6d39455adfb8d8151274/</t>
+  </si>
+  <si>
     <t>https://www.allsouth.org/</t>
   </si>
   <si>
+    <t>4.72</t>
+  </si>
+  <si>
+    <t>https://www.webpagetest.org/result/181206_K4_b9b1d866023ee222fd8d18bb8bc32dcc/</t>
+  </si>
+  <si>
     <t>https://www.rutheckerdhall.com/</t>
   </si>
   <si>
+    <t>13.27</t>
+  </si>
+  <si>
+    <t>https://www.webpagetest.org/result/181206_TE_fa85411fde4cd0121b7e684295a21ade/</t>
+  </si>
+  <si>
     <t>https://www.shelbyvote.com/</t>
   </si>
   <si>
+    <t>8.02</t>
+  </si>
+  <si>
+    <t>https://www.webpagetest.org/result/181206_E5_04bb12a04cb0c5b8be061b982c9d4cfa/</t>
+  </si>
+  <si>
     <t>https://how.drsusanloveresearch.org</t>
   </si>
   <si>
+    <t>3.44</t>
+  </si>
+  <si>
+    <t>https://www.webpagetest.org/result/181206_Y3_8d13be0a6473aeb799c56eb23b44ceaf/</t>
+  </si>
+  <si>
     <t>http://gefen.com/</t>
   </si>
   <si>
+    <t>2.58</t>
+  </si>
+  <si>
+    <t>https://www.webpagetest.org/result/181206_4R_d9da7be055a3a165ef923bcb84a18fa4/</t>
+  </si>
+  <si>
     <t>https://www.valleymetro.org/</t>
   </si>
   <si>
+    <t>5.36</t>
+  </si>
+  <si>
+    <t>https://www.webpagetest.org/result/181206_CA_e83144fe7643be7ff46d74913481c8a0/</t>
+  </si>
+  <si>
     <t>https://www.lbcc.edu/</t>
   </si>
   <si>
+    <t>4.86</t>
+  </si>
+  <si>
+    <t>https://www.webpagetest.org/result/181206_71_9ab5b0dc16dfe2ea8340647bd3e013cd/</t>
+  </si>
+  <si>
     <t>Page size</t>
   </si>
   <si>
@@ -231,60 +291,6 @@
   </si>
   <si>
     <t>5,610</t>
-  </si>
-  <si>
-    <t>https://www.webpagetest.org/result/181206_4S_45876082867661b6b0310f16516e8c40/</t>
-  </si>
-  <si>
-    <t>3.61</t>
-  </si>
-  <si>
-    <t>https://www.webpagetest.org/result/181206_36_99d5ef8dcecd71e31ece19ae15e35f0e/</t>
-  </si>
-  <si>
-    <t>2.41</t>
-  </si>
-  <si>
-    <t>https://www.webpagetest.org/result/181206_QT_2edce564946c6d39455adfb8d8151274/</t>
-  </si>
-  <si>
-    <t>4.39</t>
-  </si>
-  <si>
-    <t>https://www.webpagetest.org/result/181206_K4_b9b1d866023ee222fd8d18bb8bc32dcc/</t>
-  </si>
-  <si>
-    <t>4.72</t>
-  </si>
-  <si>
-    <t>https://www.webpagetest.org/result/181206_TE_fa85411fde4cd0121b7e684295a21ade/</t>
-  </si>
-  <si>
-    <t>13.27</t>
-  </si>
-  <si>
-    <t>https://www.webpagetest.org/result/181206_E5_04bb12a04cb0c5b8be061b982c9d4cfa/</t>
-  </si>
-  <si>
-    <t>8.02</t>
-  </si>
-  <si>
-    <t>https://www.webpagetest.org/result/181206_Y3_8d13be0a6473aeb799c56eb23b44ceaf/</t>
-  </si>
-  <si>
-    <t>3.44</t>
-  </si>
-  <si>
-    <t>https://www.webpagetest.org/result/181206_4R_d9da7be055a3a165ef923bcb84a18fa4/</t>
-  </si>
-  <si>
-    <t>2.58</t>
-  </si>
-  <si>
-    <t>https://www.webpagetest.org/result/181206_71_9ab5b0dc16dfe2ea8340647bd3e013cd/</t>
-  </si>
-  <si>
-    <t>4.86</t>
   </si>
 </sst>
 </file>
@@ -292,10 +298,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ &quot;₹&quot;\ * #,##0_ ;_ &quot;₹&quot;\ * \-#,##0_ ;_ &quot;₹&quot;\ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="_ &quot;₹&quot;\ * #,##0.00_ ;_ &quot;₹&quot;\ * \-#,##0.00_ ;_ &quot;₹&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="179" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_ &quot;₹&quot;\ * #,##0_ ;_ &quot;₹&quot;\ * \-#,##0_ ;_ &quot;₹&quot;\ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;\ * #,##0.00_ ;_ &quot;₹&quot;\ * \-#,##0.00_ ;_ &quot;₹&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="22">
     <font>
@@ -320,15 +326,24 @@
       <charset val="134"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -342,14 +357,39 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
-      <sz val="13"/>
+      <sz val="18"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
@@ -357,16 +397,16 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -380,25 +420,22 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -413,38 +450,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -458,7 +464,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -485,187 +491,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -707,17 +713,26 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF7F7F7F"/>
       </left>
       <right style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF7F7F7F"/>
       </right>
       <top style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF7F7F7F"/>
       </top>
       <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -739,18 +754,11 @@
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="medium">
+      <top style="thin">
         <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
+      </top>
       <bottom style="double">
-        <color rgb="FFFF8001"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -771,27 +779,25 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FFB2B2B2"/>
       </left>
       <right style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FFB2B2B2"/>
       </right>
       <top style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FFB2B2B2"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
+      <top/>
       <bottom style="double">
-        <color theme="4"/>
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -806,229 +812,229 @@
     </border>
   </borders>
   <cellStyleXfs count="49">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="14" fontId="4" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="0" numFmtId="177">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="0" numFmtId="179">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="0" numFmtId="176">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="0" numFmtId="178">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="0" numFmtId="9">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyNumberFormat="0" applyProtection="0" borderId="4" fillId="8" fontId="5" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="5" fillId="0" fontId="6" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyFont="0" applyNumberFormat="0" applyProtection="0" borderId="3" fillId="7" fontId="0" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="12" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="21" fontId="3" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="8" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="26" fontId="4" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="15" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="18" fontId="4" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="11" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="16" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="5" fillId="0" fontId="14" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="10" fillId="0" fontId="10" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="10" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyNumberFormat="0" applyProtection="0" borderId="8" fillId="34" fontId="21" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="11" fontId="3" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="33" fontId="20" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyNumberFormat="0" applyProtection="0" borderId="7" fillId="17" fontId="13" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="20" fontId="4" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyNumberFormat="0" applyProtection="0" borderId="8" fillId="17" fontId="17" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="6" fillId="0" fontId="7" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="9" fillId="0" fontId="19" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="13" fontId="9" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="29" fontId="18" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="6" fontId="3" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="5" fontId="4" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="12" fontId="3" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="4" fontId="3" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="32" fontId="4" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="25" fontId="4" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="10" fontId="3" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="28" fontId="3" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="19" fontId="4" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="9" fontId="3" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="27" fontId="4" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="24" fontId="4" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="31" fontId="3" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="16" fontId="4" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="30" fontId="3" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="15" fontId="3" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="23" fontId="4" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="22" fontId="3" numFmtId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
   <cellXfs count="7">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="1" fillId="2" fontId="1" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="2" fillId="2" fontId="1" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="2" numFmtId="9" xfId="0">
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="1" fillId="3" fontId="2" numFmtId="9" xfId="0">
+    <xf numFmtId="9" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
-    <cellStyle builtinId="31" name="40% - Accent1" xfId="1"/>
-    <cellStyle builtinId="3" name="Comma" xfId="2"/>
-    <cellStyle builtinId="6" name="Comma [0]" xfId="3"/>
-    <cellStyle builtinId="7" name="Currency [0]" xfId="4"/>
-    <cellStyle builtinId="4" name="Currency" xfId="5"/>
-    <cellStyle builtinId="5" name="Percent" xfId="6"/>
-    <cellStyle builtinId="23" name="Check Cell" xfId="7"/>
-    <cellStyle builtinId="17" name="Heading 2" xfId="8"/>
-    <cellStyle builtinId="10" name="Note" xfId="9"/>
-    <cellStyle builtinId="8" name="Hyperlink" xfId="10"/>
-    <cellStyle builtinId="44" name="60% - Accent4" xfId="11"/>
-    <cellStyle builtinId="9" name="Followed Hyperlink" xfId="12"/>
-    <cellStyle builtinId="39" name="40% - Accent3" xfId="13"/>
-    <cellStyle builtinId="11" name="Warning Text" xfId="14"/>
-    <cellStyle builtinId="35" name="40% - Accent2" xfId="15"/>
-    <cellStyle builtinId="15" name="Title" xfId="16"/>
-    <cellStyle builtinId="53" name="CExplanatory Text" xfId="17"/>
-    <cellStyle builtinId="16" name="Heading 1" xfId="18"/>
-    <cellStyle builtinId="18" name="Heading 3" xfId="19"/>
-    <cellStyle builtinId="19" name="Heading 4" xfId="20"/>
-    <cellStyle builtinId="20" name="Input" xfId="21"/>
-    <cellStyle builtinId="40" name="60% - Accent3" xfId="22"/>
-    <cellStyle builtinId="26" name="Good" xfId="23"/>
-    <cellStyle builtinId="21" name="Output" xfId="24"/>
-    <cellStyle builtinId="30" name="20% - Accent1" xfId="25"/>
-    <cellStyle builtinId="22" name="Calculation" xfId="26"/>
-    <cellStyle builtinId="24" name="Linked Cell" xfId="27"/>
-    <cellStyle builtinId="25" name="Total" xfId="28"/>
-    <cellStyle builtinId="27" name="Bad" xfId="29"/>
-    <cellStyle builtinId="28" name="Neutral" xfId="30"/>
-    <cellStyle builtinId="29" name="Accent1" xfId="31"/>
-    <cellStyle builtinId="46" name="20% - Accent5" xfId="32"/>
-    <cellStyle builtinId="32" name="60% - Accent1" xfId="33"/>
-    <cellStyle builtinId="33" name="Accent2" xfId="34"/>
-    <cellStyle builtinId="34" name="20% - Accent2" xfId="35"/>
-    <cellStyle builtinId="50" name="20% - Accent6" xfId="36"/>
-    <cellStyle builtinId="36" name="60% - Accent2" xfId="37"/>
-    <cellStyle builtinId="37" name="Accent3" xfId="38"/>
-    <cellStyle builtinId="38" name="20% - Accent3" xfId="39"/>
-    <cellStyle builtinId="41" name="Accent4" xfId="40"/>
-    <cellStyle builtinId="42" name="20% - Accent4" xfId="41"/>
-    <cellStyle builtinId="43" name="40% - Accent4" xfId="42"/>
-    <cellStyle builtinId="45" name="Accent5" xfId="43"/>
-    <cellStyle builtinId="47" name="40% - Accent5" xfId="44"/>
-    <cellStyle builtinId="48" name="60% - Accent5" xfId="45"/>
-    <cellStyle builtinId="49" name="Accent6" xfId="46"/>
-    <cellStyle builtinId="51" name="40% - Accent6" xfId="47"/>
-    <cellStyle builtinId="52" name="60% - Accent6" xfId="48"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="40% - Accent1" xfId="1" builtinId="31"/>
+    <cellStyle name="Comma" xfId="2" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="3" builtinId="6"/>
+    <cellStyle name="Currency [0]" xfId="4" builtinId="7"/>
+    <cellStyle name="Currency" xfId="5" builtinId="4"/>
+    <cellStyle name="Percent" xfId="6" builtinId="5"/>
+    <cellStyle name="Check Cell" xfId="7" builtinId="23"/>
+    <cellStyle name="Heading 2" xfId="8" builtinId="17"/>
+    <cellStyle name="Note" xfId="9" builtinId="10"/>
+    <cellStyle name="Hyperlink" xfId="10" builtinId="8"/>
+    <cellStyle name="60% - Accent4" xfId="11" builtinId="44"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9"/>
+    <cellStyle name="40% - Accent3" xfId="13" builtinId="39"/>
+    <cellStyle name="Warning Text" xfId="14" builtinId="11"/>
+    <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
+    <cellStyle name="Title" xfId="16" builtinId="15"/>
+    <cellStyle name="CExplanatory Text" xfId="17" builtinId="53"/>
+    <cellStyle name="Heading 1" xfId="18" builtinId="16"/>
+    <cellStyle name="Heading 3" xfId="19" builtinId="18"/>
+    <cellStyle name="Heading 4" xfId="20" builtinId="19"/>
+    <cellStyle name="Input" xfId="21" builtinId="20"/>
+    <cellStyle name="60% - Accent3" xfId="22" builtinId="40"/>
+    <cellStyle name="Good" xfId="23" builtinId="26"/>
+    <cellStyle name="Output" xfId="24" builtinId="21"/>
+    <cellStyle name="20% - Accent1" xfId="25" builtinId="30"/>
+    <cellStyle name="Calculation" xfId="26" builtinId="22"/>
+    <cellStyle name="Linked Cell" xfId="27" builtinId="24"/>
+    <cellStyle name="Total" xfId="28" builtinId="25"/>
+    <cellStyle name="Bad" xfId="29" builtinId="27"/>
+    <cellStyle name="Neutral" xfId="30" builtinId="28"/>
+    <cellStyle name="Accent1" xfId="31" builtinId="29"/>
+    <cellStyle name="20% - Accent5" xfId="32" builtinId="46"/>
+    <cellStyle name="60% - Accent1" xfId="33" builtinId="32"/>
+    <cellStyle name="Accent2" xfId="34" builtinId="33"/>
+    <cellStyle name="20% - Accent2" xfId="35" builtinId="34"/>
+    <cellStyle name="20% - Accent6" xfId="36" builtinId="50"/>
+    <cellStyle name="60% - Accent2" xfId="37" builtinId="36"/>
+    <cellStyle name="Accent3" xfId="38" builtinId="37"/>
+    <cellStyle name="20% - Accent3" xfId="39" builtinId="38"/>
+    <cellStyle name="Accent4" xfId="40" builtinId="41"/>
+    <cellStyle name="20% - Accent4" xfId="41" builtinId="42"/>
+    <cellStyle name="40% - Accent4" xfId="42" builtinId="43"/>
+    <cellStyle name="Accent5" xfId="43" builtinId="45"/>
+    <cellStyle name="40% - Accent5" xfId="44" builtinId="47"/>
+    <cellStyle name="60% - Accent5" xfId="45" builtinId="48"/>
+    <cellStyle name="Accent6" xfId="46" builtinId="49"/>
+    <cellStyle name="40% - Accent6" xfId="47" builtinId="51"/>
+    <cellStyle name="60% - Accent6" xfId="48" builtinId="52"/>
   </cellStyles>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -1042,10 +1048,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -1209,21 +1215,21 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="6350">
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="12700">
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="19050">
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -1240,7 +1246,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw algn="ctr" blurRad="57150" dir="5400000" dist="19050" rotWithShape="0">
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -1293,9 +1299,9 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C1" sqref="C1"/>
@@ -1303,12 +1309,12 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="2"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="34.2857142857143" collapsed="false"/>
-    <col min="2" max="2" customWidth="true" width="21.2857142857143" collapsed="false"/>
-    <col min="3" max="3" customWidth="true" width="80.8571428571429" collapsed="false"/>
+    <col min="1" max="1" width="34.2857142857143" customWidth="1"/>
+    <col min="2" max="2" width="21.2857142857143" customWidth="1"/>
+    <col min="3" max="3" width="80.8571428571429" customWidth="1"/>
   </cols>
   <sheetData>
-    <row ht="30" r="1" spans="1:3">
+    <row r="1" ht="30" spans="1:3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1324,117 +1330,121 @@
         <v>3</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>72</v>
+        <v>4</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>71</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="2" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>74</v>
+        <v>7</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>73</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="2" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>76</v>
+        <v>10</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>75</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="2" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>78</v>
+        <v>13</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>77</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="2" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>80</v>
+        <v>16</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>79</v>
+        <v>17</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="2" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>82</v>
+        <v>19</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>81</v>
+        <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" s="2" t="s">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>84</v>
+        <v>22</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>83</v>
+        <v>23</v>
       </c>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" s="2" t="s">
-        <v>10</v>
+        <v>24</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>86</v>
+        <v>25</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>85</v>
+        <v>26</v>
       </c>
     </row>
     <row r="10" spans="1:3">
       <c r="A10" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B10" s="3"/>
-      <c r="C10" s="2"/>
+        <v>27</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="11" spans="1:3">
       <c r="A11" s="2" t="s">
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>88</v>
+        <v>31</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>87</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.511805555555556" header="0.511805555555556" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
   <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1442,28 +1452,28 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="4"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="37.5714285714286" collapsed="false"/>
-    <col min="2" max="2" customWidth="true" width="9.85714285714286" collapsed="false"/>
-    <col min="3" max="3" customWidth="true" width="8.85714285714286" collapsed="false"/>
-    <col min="4" max="4" customWidth="true" width="14.0" collapsed="false"/>
-    <col min="5" max="5" customWidth="true" width="89.2857142857143" collapsed="false"/>
+    <col min="1" max="1" width="37.5714285714286" customWidth="1"/>
+    <col min="2" max="2" width="9.85714285714286" customWidth="1"/>
+    <col min="3" max="3" width="8.85714285714286" customWidth="1"/>
+    <col min="4" max="4" width="14" customWidth="1"/>
+    <col min="5" max="5" width="89.2857142857143" customWidth="1"/>
   </cols>
   <sheetData>
-    <row ht="30" r="1" spans="1:5">
+    <row r="1" ht="30" spans="1:5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>13</v>
+        <v>33</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>14</v>
+        <v>34</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>15</v>
+        <v>35</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>16</v>
+        <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -1471,190 +1481,190 @@
         <v>3</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>17</v>
+        <v>37</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>18</v>
+        <v>38</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>19</v>
+        <v>39</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>20</v>
+        <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="2" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>21</v>
+        <v>41</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>22</v>
+        <v>42</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>23</v>
+        <v>43</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>24</v>
+        <v>44</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="2" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>25</v>
+        <v>45</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>26</v>
+        <v>46</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>27</v>
+        <v>47</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>28</v>
+        <v>48</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" s="2" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>29</v>
+        <v>49</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>30</v>
+        <v>50</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>31</v>
+        <v>51</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>32</v>
+        <v>52</v>
       </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" s="2" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>33</v>
+        <v>53</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>34</v>
+        <v>54</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>35</v>
+        <v>55</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>36</v>
+        <v>56</v>
       </c>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" s="2" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>37</v>
+        <v>57</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>38</v>
+        <v>58</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>39</v>
+        <v>59</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>40</v>
+        <v>60</v>
       </c>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" s="2" t="s">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>41</v>
+        <v>61</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>42</v>
+        <v>62</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>43</v>
+        <v>63</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>44</v>
+        <v>64</v>
       </c>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" s="2" t="s">
-        <v>10</v>
+        <v>24</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>45</v>
+        <v>65</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>46</v>
+        <v>66</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>47</v>
+        <v>67</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>48</v>
+        <v>68</v>
       </c>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" s="2" t="s">
-        <v>11</v>
+        <v>27</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>49</v>
+        <v>69</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>50</v>
+        <v>70</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>51</v>
+        <v>71</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>52</v>
+        <v>72</v>
       </c>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" s="2" t="s">
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>53</v>
+        <v>73</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>54</v>
+        <v>74</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>55</v>
+        <v>75</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>56</v>
+        <v>76</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.511805555555556" header="0.511805555555556" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
   <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="3" outlineLevelRow="7"/>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="7" outlineLevelCol="3"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="37.5714285714286" collapsed="false"/>
-    <col min="3" max="3" customWidth="true" width="12.2857142857143" collapsed="false"/>
+    <col min="1" max="1" width="37.5714285714286" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="12.2857142857143" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -1662,10 +1672,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>57</v>
+        <v>77</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>58</v>
+        <v>78</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -1675,73 +1685,73 @@
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
       <c r="D2" t="s">
-        <v>59</v>
+        <v>79</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="2" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B3" s="5"/>
       <c r="C3" s="5"/>
       <c r="D3" t="s">
-        <v>59</v>
+        <v>79</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="2" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="B4" s="5"/>
       <c r="C4" s="5"/>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="2" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="B5" s="5"/>
       <c r="C5" s="5"/>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="2" t="s">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="B6" s="6"/>
       <c r="C6" s="5"/>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="2" t="s">
-        <v>10</v>
+        <v>24</v>
       </c>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" s="2" t="s">
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.511805555555556" header="0.511805555555556" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
   <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="1"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="37.5714285714286" collapsed="false"/>
-    <col min="2" max="2" customWidth="true" width="13.2857142857143" collapsed="false"/>
+    <col min="1" max="1" width="37.5714285714286" customWidth="1"/>
+    <col min="2" max="2" width="13.2857142857143" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -1749,7 +1759,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>60</v>
+        <v>80</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -1757,83 +1767,83 @@
         <v>3</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>61</v>
+        <v>81</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="2" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>62</v>
+        <v>82</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="2" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>63</v>
+        <v>83</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="2" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>64</v>
+        <v>84</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="2" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>65</v>
+        <v>85</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" s="2" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>66</v>
+        <v>86</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" s="2" t="s">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>67</v>
+        <v>87</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" s="2" t="s">
-        <v>10</v>
+        <v>24</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>68</v>
+        <v>88</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" s="2" t="s">
-        <v>11</v>
+        <v>27</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>69</v>
+        <v>89</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" s="2" t="s">
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>70</v>
+        <v>90</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.511805555555556" header="0.511805555555556" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
   <headerFooter/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Committed on 07:12:2018:12:51:00PM By Karthikeyan Rajendran
</commit_message>
<xml_diff>
--- a/data/Performance_Audit.xlsx
+++ b/data/Performance_Audit.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="20295" windowHeight="8340" activeTab="4"/>
+    <workbookView windowWidth="20385" windowHeight="8370" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Web_Page_Test_Mobile" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51">
   <si>
     <t>Urls</t>
   </si>
@@ -91,6 +91,87 @@
   </si>
   <si>
     <t>URL</t>
+  </si>
+  <si>
+    <t>F(32%)</t>
+  </si>
+  <si>
+    <t>D(65%)</t>
+  </si>
+  <si>
+    <t>https://gtmetrix.com/reports/www.sfwmd.gov/QXNTpbHt</t>
+  </si>
+  <si>
+    <t>A(92%)</t>
+  </si>
+  <si>
+    <t>B(83%)</t>
+  </si>
+  <si>
+    <t>https://gtmetrix.com/reports/www.nicb.org/ODOZ4yyE</t>
+  </si>
+  <si>
+    <t>F(27%)</t>
+  </si>
+  <si>
+    <t>B(84%)</t>
+  </si>
+  <si>
+    <t>https://gtmetrix.com/reports/www.boston.gov/Je4BaCPb</t>
+  </si>
+  <si>
+    <t>F(13%)</t>
+  </si>
+  <si>
+    <t>https://gtmetrix.com/reports/www.allsouth.org/pofOIELM</t>
+  </si>
+  <si>
+    <t>F(35%)</t>
+  </si>
+  <si>
+    <t>F(49%)</t>
+  </si>
+  <si>
+    <t>https://gtmetrix.com/reports/www.rutheckerdhall.com/NV2NIPni</t>
+  </si>
+  <si>
+    <t>E(50%)</t>
+  </si>
+  <si>
+    <t>E(55%)</t>
+  </si>
+  <si>
+    <t>https://gtmetrix.com/reports/www.shelbyvote.com/bXGZAROT</t>
+  </si>
+  <si>
+    <t>B(87%)</t>
+  </si>
+  <si>
+    <t>D(64%)</t>
+  </si>
+  <si>
+    <t>https://gtmetrix.com/reports/how.drsusanloveresearch.org/w6DILNfU</t>
+  </si>
+  <si>
+    <t>C(74%)</t>
+  </si>
+  <si>
+    <t>https://gtmetrix.com/reports/gefen.com/g6cCx9jJ</t>
+  </si>
+  <si>
+    <t>E(59%)</t>
+  </si>
+  <si>
+    <t>D(63%)</t>
+  </si>
+  <si>
+    <t>https://gtmetrix.com/reports/www.valleymetro.org/kJ6fyeBN</t>
+  </si>
+  <si>
+    <t>E(58%)</t>
+  </si>
+  <si>
+    <t>https://gtmetrix.com/reports/www.lbcc.edu/X6bh6g65</t>
   </si>
 </sst>
 </file>
@@ -98,8 +179,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="178" formatCode="_ &quot;₹&quot;\ * #,##0_ ;_ &quot;₹&quot;\ * \-#,##0_ ;_ &quot;₹&quot;\ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;\ * #,##0.00_ ;_ &quot;₹&quot;\ * \-#,##0.00_ ;_ &quot;₹&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
@@ -133,6 +214,135 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="18"/>
       <color theme="3"/>
@@ -140,135 +350,6 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="35">
     <fill>
@@ -291,187 +372,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -513,6 +594,21 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -524,6 +620,30 @@
       </top>
       <bottom style="double">
         <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -547,22 +667,7 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -586,44 +691,20 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
@@ -633,134 +714,134 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="24" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="31" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="13" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="19" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="19" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -772,6 +853,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1348,13 +1432,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="5" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1372,8 +1456,8 @@
       <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="5"/>
-      <c r="C3" s="5"/>
+      <c r="B3" s="6"/>
+      <c r="C3" s="6"/>
       <c r="D3" t="s">
         <v>19</v>
       </c>
@@ -1382,22 +1466,22 @@
       <c r="A4" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="5"/>
-      <c r="C4" s="5"/>
+      <c r="B4" s="6"/>
+      <c r="C4" s="6"/>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="5"/>
-      <c r="C5" s="5"/>
+      <c r="B5" s="6"/>
+      <c r="C5" s="6"/>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="6"/>
-      <c r="C6" s="5"/>
+      <c r="B6" s="7"/>
+      <c r="C6" s="6"/>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="2" t="s">
@@ -1514,15 +1598,15 @@
   <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="3"/>
   <cols>
     <col min="1" max="1" width="37.5714285714286" customWidth="1"/>
-    <col min="2" max="2" width="16.2857142857143" customWidth="1"/>
-    <col min="3" max="3" width="15.4285714285714" customWidth="1"/>
-    <col min="4" max="4" width="17.4285714285714" customWidth="1"/>
+    <col min="2" max="2" width="12.2857142857143" customWidth="1"/>
+    <col min="3" max="3" width="11.1428571428571" customWidth="1"/>
+    <col min="4" max="4" width="65" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="21" customHeight="1" spans="1:4">
@@ -1543,81 +1627,141 @@
       <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
+      <c r="B2" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
+      <c r="B3" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
+      <c r="B4" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
+      <c r="B5" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
+      <c r="B6" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
+      <c r="B7" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="3"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
+      <c r="B8" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="3"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
+      <c r="B9" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B10" s="3"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
+      <c r="B10" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B11" s="3"/>
-      <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
+      <c r="B11" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>50</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>

</xml_diff>

<commit_message>
mobile friendly site updated in process automation script on 07.12.2018.15.08
</commit_message>
<xml_diff>
--- a/data/Performance_Audit.xlsx
+++ b/data/Performance_Audit.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="20385" windowHeight="8370" activeTab="4"/>
+    <workbookView windowWidth="20295" windowHeight="8340" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Web_Page_Test_Mobile" sheetId="1" r:id="rId1"/>
@@ -12,6 +12,7 @@
     <sheet name="Page_Insight" sheetId="3" r:id="rId3"/>
     <sheet name="Page_Count" sheetId="4" r:id="rId4"/>
     <sheet name="GT_metrix" sheetId="5" r:id="rId5"/>
+    <sheet name="Mobile_friendly" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="144525"/>
   <oleSize ref="A1:C11"/>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53">
   <si>
     <t>Urls</t>
   </si>
@@ -172,6 +173,12 @@
   </si>
   <si>
     <t>https://gtmetrix.com/reports/www.lbcc.edu/X6bh6g65</t>
+  </si>
+  <si>
+    <t>Result</t>
+  </si>
+  <si>
+    <t>Resulturl</t>
   </si>
 </sst>
 </file>
@@ -180,9 +187,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ &quot;₹&quot;\ * #,##0.00_ ;_ &quot;₹&quot;\ * \-#,##0.00_ ;_ &quot;₹&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="178" formatCode="_ &quot;₹&quot;\ * #,##0_ ;_ &quot;₹&quot;\ * \-#,##0_ ;_ &quot;₹&quot;\ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;\ * #,##0.00_ ;_ &quot;₹&quot;\ * \-#,##0.00_ ;_ &quot;₹&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="22">
     <font>
@@ -221,6 +228,45 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
@@ -229,11 +275,10 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -245,8 +290,17 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -261,30 +315,22 @@
     </font>
     <font>
       <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -298,44 +344,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
@@ -343,11 +351,10 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -372,187 +379,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -575,9 +582,7 @@
       <top style="thin">
         <color auto="1"/>
       </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
+      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -590,21 +595,17 @@
       <top style="thin">
         <color auto="1"/>
       </top>
-      <bottom/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -624,15 +625,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -644,6 +636,15 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -663,11 +664,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -696,148 +703,148 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="23" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="16" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="16" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="13" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -848,23 +855,23 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="2" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="9" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
@@ -1199,13 +1206,13 @@
   </cols>
   <sheetData>
     <row r="1" ht="30" spans="1:3">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="6" t="s">
         <v>2</v>
       </c>
     </row>
@@ -1304,19 +1311,19 @@
   </cols>
   <sheetData>
     <row r="1" ht="30" spans="1:5">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="6" t="s">
         <v>16</v>
       </c>
     </row>
@@ -1422,7 +1429,7 @@
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="A1" sqref="A1:C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="7" outlineLevelCol="3"/>
@@ -1432,13 +1439,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="1" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1456,8 +1463,8 @@
       <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="6"/>
-      <c r="C3" s="6"/>
+      <c r="B3" s="4"/>
+      <c r="C3" s="4"/>
       <c r="D3" t="s">
         <v>19</v>
       </c>
@@ -1466,22 +1473,22 @@
       <c r="A4" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="6"/>
-      <c r="C4" s="6"/>
+      <c r="B4" s="4"/>
+      <c r="C4" s="4"/>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="6"/>
-      <c r="C5" s="6"/>
+      <c r="B5" s="4"/>
+      <c r="C5" s="4"/>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="7"/>
-      <c r="C6" s="6"/>
+      <c r="B6" s="5"/>
+      <c r="C6" s="4"/>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="2" t="s">
@@ -1519,10 +1526,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="6" t="s">
         <v>20</v>
       </c>
     </row>
@@ -1597,8 +1604,8 @@
   <sheetPr/>
   <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1:A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="3"/>
@@ -1610,16 +1617,16 @@
   </cols>
   <sheetData>
     <row r="1" ht="21" customHeight="1" spans="1:4">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="6" t="s">
         <v>23</v>
       </c>
     </row>
@@ -1633,7 +1640,7 @@
       <c r="C2" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="7" t="s">
         <v>26</v>
       </c>
     </row>
@@ -1647,7 +1654,7 @@
       <c r="C3" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D3" s="7" t="s">
         <v>29</v>
       </c>
     </row>
@@ -1661,7 +1668,7 @@
       <c r="C4" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="D4" s="7" t="s">
         <v>32</v>
       </c>
     </row>
@@ -1675,7 +1682,7 @@
       <c r="C5" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="D5" s="7" t="s">
         <v>34</v>
       </c>
     </row>
@@ -1689,7 +1696,7 @@
       <c r="C6" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="D6" s="4" t="s">
+      <c r="D6" s="7" t="s">
         <v>37</v>
       </c>
     </row>
@@ -1703,7 +1710,7 @@
       <c r="C7" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="D7" s="4" t="s">
+      <c r="D7" s="7" t="s">
         <v>40</v>
       </c>
     </row>
@@ -1717,7 +1724,7 @@
       <c r="C8" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="D8" s="4" t="s">
+      <c r="D8" s="7" t="s">
         <v>43</v>
       </c>
     </row>
@@ -1731,7 +1738,7 @@
       <c r="C9" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="D9" s="4" t="s">
+      <c r="D9" s="7" t="s">
         <v>45</v>
       </c>
     </row>
@@ -1745,7 +1752,7 @@
       <c r="C10" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="D10" s="4" t="s">
+      <c r="D10" s="7" t="s">
         <v>48</v>
       </c>
     </row>
@@ -1759,9 +1766,91 @@
       <c r="C11" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="D11" s="4" t="s">
+      <c r="D11" s="7" t="s">
         <v>50</v>
       </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:C8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="7" outlineLevelCol="2"/>
+  <cols>
+    <col min="1" max="1" width="37.5714285714286" customWidth="1"/>
+    <col min="2" max="2" width="6.28571428571429" customWidth="1"/>
+    <col min="3" max="3" width="8.71428571428571" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="3"/>
+      <c r="C2" s="3"/>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="4"/>
+      <c r="C3" s="4"/>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="4"/>
+      <c r="C4" s="4"/>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="4"/>
+      <c r="C5" s="4"/>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="5"/>
+      <c r="C6" s="4"/>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" s="3"/>
+      <c r="C8" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>

</xml_diff>

<commit_message>
Committed on 10:12:2018:16:00:00PM By Karthikeyan Rajendran
</commit_message>
<xml_diff>
--- a/data/Performance_Audit.xlsx
+++ b/data/Performance_Audit.xlsx
@@ -4,15 +4,15 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="20295" windowHeight="8340" activeTab="5"/>
+    <workbookView activeTab="5" windowHeight="8340" windowWidth="20295"/>
   </bookViews>
   <sheets>
-    <sheet name="Web_Page_Test_Mobile" sheetId="1" r:id="rId1"/>
-    <sheet name="Web_Page_Test_Desktop" sheetId="2" r:id="rId2"/>
-    <sheet name="Page_Insight" sheetId="3" r:id="rId3"/>
-    <sheet name="Page_Count" sheetId="4" r:id="rId4"/>
-    <sheet name="GT_metrix" sheetId="5" r:id="rId5"/>
-    <sheet name="Mobile_friendly" sheetId="6" r:id="rId6"/>
+    <sheet name="Web_Page_Test_Mobile" r:id="rId1" sheetId="1"/>
+    <sheet name="Web_Page_Test_Desktop" r:id="rId2" sheetId="2"/>
+    <sheet name="Page_Insight" r:id="rId3" sheetId="3"/>
+    <sheet name="Page_Count" r:id="rId4" sheetId="4"/>
+    <sheet name="GT_metrix" r:id="rId5" sheetId="5"/>
+    <sheet name="Mobile_friendly" r:id="rId6" sheetId="6"/>
   </sheets>
   <calcPr calcId="144525"/>
   <oleSize ref="A1:C11"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="72">
   <si>
     <t>Urls</t>
   </si>
@@ -179,6 +179,222 @@
   </si>
   <si>
     <t>Resulturl</t>
+  </si>
+  <si>
+    <t>43%</t>
+  </si>
+  <si>
+    <t>97%</t>
+  </si>
+  <si>
+    <t>83%</t>
+  </si>
+  <si>
+    <t>99%</t>
+  </si>
+  <si>
+    <t>68%</t>
+  </si>
+  <si>
+    <t>75%</t>
+  </si>
+  <si>
+    <t>20%</t>
+  </si>
+  <si>
+    <t>77%</t>
+  </si>
+  <si>
+    <t>15%</t>
+  </si>
+  <si>
+    <t>65%</t>
+  </si>
+  <si>
+    <t>88%</t>
+  </si>
+  <si>
+    <t>100%</t>
+  </si>
+  <si>
+    <t>40%</t>
+  </si>
+  <si>
+    <t>95%</t>
+  </si>
+  <si>
+    <t>https://gtmetrix.com/reports/www.sfwmd.gov/nh6xdrVt</t>
+  </si>
+  <si>
+    <t>https://gtmetrix.com/reports/www.nicb.org/rltIgEyq</t>
+  </si>
+  <si>
+    <t>https://gtmetrix.com/reports/www.boston.gov/SxjYTOdu</t>
+  </si>
+  <si>
+    <t>https://gtmetrix.com/reports/www.allsouth.org/phpDMxu9</t>
+  </si>
+  <si>
+    <t>https://gtmetrix.com/reports/www.rutheckerdhall.com/6HlVwutx</t>
+  </si>
+  <si>
+    <t>F(36%)</t>
+  </si>
+  <si>
+    <t>https://gtmetrix.com/reports/www.shelbyvote.com/wCnyuHP2</t>
+  </si>
+  <si>
+    <t>https://gtmetrix.com/reports/how.drsusanloveresearch.org/050XH35u</t>
+  </si>
+  <si>
+    <t>https://gtmetrix.com/reports/gefen.com/DHAGuRSq</t>
+  </si>
+  <si>
+    <t>https://gtmetrix.com/reports/www.valleymetro.org/nnPRsM6K</t>
+  </si>
+  <si>
+    <t>D(62%)</t>
+  </si>
+  <si>
+    <t>https://gtmetrix.com/reports/www.lbcc.edu/csos1QAR</t>
+  </si>
+  <si>
+    <t>https://www.webpagetest.org/result/181210_TR_07200f22b27af59b30d63b53dbb9762f/</t>
+  </si>
+  <si>
+    <t>3.63</t>
+  </si>
+  <si>
+    <t>https://www.webpagetest.org/result/181210_4A_db10921b332d169f07000a2f850e7e90/</t>
+  </si>
+  <si>
+    <t>12.02</t>
+  </si>
+  <si>
+    <t>https://www.webpagetest.org/result/181210_Z7_2edc47cdad1df063987509135ce435f4/</t>
+  </si>
+  <si>
+    <t>2.58</t>
+  </si>
+  <si>
+    <t>https://www.webpagetest.org/result/181210_XX_b4c648677c039f653c73c864cff976db/</t>
+  </si>
+  <si>
+    <t>5.66</t>
+  </si>
+  <si>
+    <t>https://www.webpagetest.org/result/181210_T4_1f0b1239d3f016e9c17b0e31b669aa63/</t>
+  </si>
+  <si>
+    <t>4.78</t>
+  </si>
+  <si>
+    <t>https://www.webpagetest.org/result/181210_NA_a3bf799fa5ff8bc79964d45d9fd26092/</t>
+  </si>
+  <si>
+    <t>6.69</t>
+  </si>
+  <si>
+    <t>107</t>
+  </si>
+  <si>
+    <t>3,510 KB</t>
+  </si>
+  <si>
+    <t>https://www.webpagetest.org/result/181210_VG_1e4104ac9a9e88cded2a543137f5095b/</t>
+  </si>
+  <si>
+    <t>3.28</t>
+  </si>
+  <si>
+    <t>63</t>
+  </si>
+  <si>
+    <t>1,352 KB</t>
+  </si>
+  <si>
+    <t>https://www.webpagetest.org/result/181210_78_85685bea83491c275066b23ed5d3b7cf/</t>
+  </si>
+  <si>
+    <t>8.64</t>
+  </si>
+  <si>
+    <t>87</t>
+  </si>
+  <si>
+    <t>4,607 KB</t>
+  </si>
+  <si>
+    <t>https://www.webpagetest.org/result/181210_QT_3cdeb279d4d849c2ef21569a2f98dabe/</t>
+  </si>
+  <si>
+    <t>27.04</t>
+  </si>
+  <si>
+    <t>218</t>
+  </si>
+  <si>
+    <t>14,585 KB</t>
+  </si>
+  <si>
+    <t>https://www.webpagetest.org/result/181210_3W_11031031fe48f0019448ebda36202a09/</t>
+  </si>
+  <si>
+    <t>11.17</t>
+  </si>
+  <si>
+    <t>155</t>
+  </si>
+  <si>
+    <t>3,978 KB</t>
+  </si>
+  <si>
+    <t>https://www.webpagetest.org/result/181210_PJ_30debc7d2674b6fee1debdbde2e750b5/</t>
+  </si>
+  <si>
+    <t>2.74</t>
+  </si>
+  <si>
+    <t>83</t>
+  </si>
+  <si>
+    <t>826 KB</t>
+  </si>
+  <si>
+    <t>https://www.webpagetest.org/result/181210_PD_706ad08b942def94d66331506b392072/</t>
+  </si>
+  <si>
+    <t>4.91</t>
+  </si>
+  <si>
+    <t>42</t>
+  </si>
+  <si>
+    <t>2,682 KB</t>
+  </si>
+  <si>
+    <t>https://www.webpagetest.org/result/181210_QY_1b1e799475a937e67a7039d660c01a21/</t>
+  </si>
+  <si>
+    <t>7.28</t>
+  </si>
+  <si>
+    <t>134</t>
+  </si>
+  <si>
+    <t>3,050 KB</t>
+  </si>
+  <si>
+    <t>https://www.webpagetest.org/result/181210_W7_c17210311871a93c3d3860aeaa2ca9a7/</t>
+  </si>
+  <si>
+    <t>5.79</t>
+  </si>
+  <si>
+    <t>73</t>
+  </si>
+  <si>
+    <t>2,731 KB</t>
   </si>
 </sst>
 </file>
@@ -700,232 +916,232 @@
     </border>
   </borders>
   <cellStyleXfs count="49">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="20" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="23" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="16" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="16" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="8" fontId="4" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="0" numFmtId="179">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="0" numFmtId="176">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="0" numFmtId="178">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="0" numFmtId="177">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="0" numFmtId="9">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyNumberFormat="0" applyProtection="0" borderId="4" fillId="12" fontId="10" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="3" fillId="0" fontId="6" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyFont="0" applyNumberFormat="0" applyProtection="0" borderId="8" fillId="20" fontId="0" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="14" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="11" fontId="3" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="9" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="24" fontId="4" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="5" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="7" fontId="4" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="13" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="8" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="3" fillId="0" fontId="16" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="6" fillId="0" fontId="7" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="7" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyNumberFormat="0" applyProtection="0" borderId="5" fillId="23" fontId="17" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="29" fontId="3" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="28" fontId="18" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyNumberFormat="0" applyProtection="0" borderId="7" fillId="16" fontId="15" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="6" fontId="4" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyNumberFormat="0" applyProtection="0" borderId="5" fillId="16" fontId="12" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="10" fillId="0" fontId="20" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="9" fillId="0" fontId="19" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="15" fontId="11" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="34" fontId="21" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="27" fontId="3" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="19" fontId="4" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="14" fontId="3" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="18" fontId="3" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="31" fontId="4" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="30" fontId="4" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="10" fontId="3" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="22" fontId="3" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="5" fontId="4" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="4" fontId="3" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="26" fontId="4" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="9" fontId="4" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="33" fontId="3" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="25" fontId="4" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="32" fontId="3" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="17" fontId="3" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="13" fontId="4" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="21" fontId="3" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
   <cellXfs count="8">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="1" fillId="2" fontId="1" numFmtId="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf applyBorder="1" borderId="2" fillId="0" fontId="0" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" borderId="2" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="2" fillId="0" fontId="2" numFmtId="9" xfId="0">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="9" fontId="2" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="2" fillId="3" fontId="2" numFmtId="9" xfId="0">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="2" fillId="2" fontId="1" numFmtId="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" borderId="2" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="40% - Accent1" xfId="1" builtinId="31"/>
-    <cellStyle name="Comma" xfId="2" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="3" builtinId="6"/>
-    <cellStyle name="Currency [0]" xfId="4" builtinId="7"/>
-    <cellStyle name="Currency" xfId="5" builtinId="4"/>
-    <cellStyle name="Percent" xfId="6" builtinId="5"/>
-    <cellStyle name="Check Cell" xfId="7" builtinId="23"/>
-    <cellStyle name="Heading 2" xfId="8" builtinId="17"/>
-    <cellStyle name="Note" xfId="9" builtinId="10"/>
-    <cellStyle name="Hyperlink" xfId="10" builtinId="8"/>
-    <cellStyle name="60% - Accent4" xfId="11" builtinId="44"/>
-    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9"/>
-    <cellStyle name="40% - Accent3" xfId="13" builtinId="39"/>
-    <cellStyle name="Warning Text" xfId="14" builtinId="11"/>
-    <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
-    <cellStyle name="Title" xfId="16" builtinId="15"/>
-    <cellStyle name="CExplanatory Text" xfId="17" builtinId="53"/>
-    <cellStyle name="Heading 1" xfId="18" builtinId="16"/>
-    <cellStyle name="Heading 3" xfId="19" builtinId="18"/>
-    <cellStyle name="Heading 4" xfId="20" builtinId="19"/>
-    <cellStyle name="Input" xfId="21" builtinId="20"/>
-    <cellStyle name="60% - Accent3" xfId="22" builtinId="40"/>
-    <cellStyle name="Good" xfId="23" builtinId="26"/>
-    <cellStyle name="Output" xfId="24" builtinId="21"/>
-    <cellStyle name="20% - Accent1" xfId="25" builtinId="30"/>
-    <cellStyle name="Calculation" xfId="26" builtinId="22"/>
-    <cellStyle name="Linked Cell" xfId="27" builtinId="24"/>
-    <cellStyle name="Total" xfId="28" builtinId="25"/>
-    <cellStyle name="Bad" xfId="29" builtinId="27"/>
-    <cellStyle name="Neutral" xfId="30" builtinId="28"/>
-    <cellStyle name="Accent1" xfId="31" builtinId="29"/>
-    <cellStyle name="20% - Accent5" xfId="32" builtinId="46"/>
-    <cellStyle name="60% - Accent1" xfId="33" builtinId="32"/>
-    <cellStyle name="Accent2" xfId="34" builtinId="33"/>
-    <cellStyle name="20% - Accent2" xfId="35" builtinId="34"/>
-    <cellStyle name="20% - Accent6" xfId="36" builtinId="50"/>
-    <cellStyle name="60% - Accent2" xfId="37" builtinId="36"/>
-    <cellStyle name="Accent3" xfId="38" builtinId="37"/>
-    <cellStyle name="20% - Accent3" xfId="39" builtinId="38"/>
-    <cellStyle name="Accent4" xfId="40" builtinId="41"/>
-    <cellStyle name="20% - Accent4" xfId="41" builtinId="42"/>
-    <cellStyle name="40% - Accent4" xfId="42" builtinId="43"/>
-    <cellStyle name="Accent5" xfId="43" builtinId="45"/>
-    <cellStyle name="40% - Accent5" xfId="44" builtinId="47"/>
-    <cellStyle name="60% - Accent5" xfId="45" builtinId="48"/>
-    <cellStyle name="Accent6" xfId="46" builtinId="49"/>
-    <cellStyle name="40% - Accent6" xfId="47" builtinId="51"/>
-    <cellStyle name="60% - Accent6" xfId="48" builtinId="52"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle builtinId="31" name="40% - Accent1" xfId="1"/>
+    <cellStyle builtinId="3" name="Comma" xfId="2"/>
+    <cellStyle builtinId="6" name="Comma [0]" xfId="3"/>
+    <cellStyle builtinId="7" name="Currency [0]" xfId="4"/>
+    <cellStyle builtinId="4" name="Currency" xfId="5"/>
+    <cellStyle builtinId="5" name="Percent" xfId="6"/>
+    <cellStyle builtinId="23" name="Check Cell" xfId="7"/>
+    <cellStyle builtinId="17" name="Heading 2" xfId="8"/>
+    <cellStyle builtinId="10" name="Note" xfId="9"/>
+    <cellStyle builtinId="8" name="Hyperlink" xfId="10"/>
+    <cellStyle builtinId="44" name="60% - Accent4" xfId="11"/>
+    <cellStyle builtinId="9" name="Followed Hyperlink" xfId="12"/>
+    <cellStyle builtinId="39" name="40% - Accent3" xfId="13"/>
+    <cellStyle builtinId="11" name="Warning Text" xfId="14"/>
+    <cellStyle builtinId="35" name="40% - Accent2" xfId="15"/>
+    <cellStyle builtinId="15" name="Title" xfId="16"/>
+    <cellStyle builtinId="53" name="CExplanatory Text" xfId="17"/>
+    <cellStyle builtinId="16" name="Heading 1" xfId="18"/>
+    <cellStyle builtinId="18" name="Heading 3" xfId="19"/>
+    <cellStyle builtinId="19" name="Heading 4" xfId="20"/>
+    <cellStyle builtinId="20" name="Input" xfId="21"/>
+    <cellStyle builtinId="40" name="60% - Accent3" xfId="22"/>
+    <cellStyle builtinId="26" name="Good" xfId="23"/>
+    <cellStyle builtinId="21" name="Output" xfId="24"/>
+    <cellStyle builtinId="30" name="20% - Accent1" xfId="25"/>
+    <cellStyle builtinId="22" name="Calculation" xfId="26"/>
+    <cellStyle builtinId="24" name="Linked Cell" xfId="27"/>
+    <cellStyle builtinId="25" name="Total" xfId="28"/>
+    <cellStyle builtinId="27" name="Bad" xfId="29"/>
+    <cellStyle builtinId="28" name="Neutral" xfId="30"/>
+    <cellStyle builtinId="29" name="Accent1" xfId="31"/>
+    <cellStyle builtinId="46" name="20% - Accent5" xfId="32"/>
+    <cellStyle builtinId="32" name="60% - Accent1" xfId="33"/>
+    <cellStyle builtinId="33" name="Accent2" xfId="34"/>
+    <cellStyle builtinId="34" name="20% - Accent2" xfId="35"/>
+    <cellStyle builtinId="50" name="20% - Accent6" xfId="36"/>
+    <cellStyle builtinId="36" name="60% - Accent2" xfId="37"/>
+    <cellStyle builtinId="37" name="Accent3" xfId="38"/>
+    <cellStyle builtinId="38" name="20% - Accent3" xfId="39"/>
+    <cellStyle builtinId="41" name="Accent4" xfId="40"/>
+    <cellStyle builtinId="42" name="20% - Accent4" xfId="41"/>
+    <cellStyle builtinId="43" name="40% - Accent4" xfId="42"/>
+    <cellStyle builtinId="45" name="Accent5" xfId="43"/>
+    <cellStyle builtinId="47" name="40% - Accent5" xfId="44"/>
+    <cellStyle builtinId="48" name="60% - Accent5" xfId="45"/>
+    <cellStyle builtinId="49" name="Accent6" xfId="46"/>
+    <cellStyle builtinId="51" name="40% - Accent6" xfId="47"/>
+    <cellStyle builtinId="52" name="60% - Accent6" xfId="48"/>
   </cellStyles>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -939,10 +1155,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -1106,21 +1322,21 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="6350">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="12700">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="19050">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -1137,7 +1353,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw algn="ctr" blurRad="57150" dir="5400000" dist="19050" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -1190,9 +1406,9 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <sheetPr/>
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C17" sqref="C17"/>
@@ -1200,12 +1416,12 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="2"/>
   <cols>
-    <col min="1" max="1" width="34.2857142857143" customWidth="1"/>
-    <col min="2" max="2" width="21.2857142857143" customWidth="1"/>
-    <col min="3" max="3" width="80.8571428571429" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="34.2857142857143" collapsed="false"/>
+    <col min="2" max="2" customWidth="true" width="21.2857142857143" collapsed="false"/>
+    <col min="3" max="3" customWidth="true" width="80.8571428571429" collapsed="false"/>
   </cols>
   <sheetData>
-    <row r="1" ht="30" spans="1:3">
+    <row ht="30" r="1" spans="1:3">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -1227,8 +1443,12 @@
       <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="3"/>
-      <c r="C3" s="2"/>
+      <c r="B3" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>79</v>
+      </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="2" t="s">
@@ -1248,8 +1468,12 @@
       <c r="A6" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="3"/>
-      <c r="C6" s="2"/>
+      <c r="B6" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>81</v>
+      </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="2" t="s">
@@ -1269,33 +1493,45 @@
       <c r="A9" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="3"/>
-      <c r="C9" s="2"/>
+      <c r="B9" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="10" spans="1:3">
       <c r="A10" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B10" s="3"/>
-      <c r="C10" s="2"/>
+      <c r="B10" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>85</v>
+      </c>
     </row>
     <row r="11" spans="1:3">
       <c r="A11" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B11" s="3"/>
-      <c r="C11" s="2"/>
+      <c r="B11" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>87</v>
+      </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
+  <pageMargins bottom="1" footer="0.511805555555556" header="0.511805555555556" left="0.75" right="0.75" top="1"/>
   <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <sheetPr/>
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2:E11"/>
@@ -1303,14 +1539,14 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="4"/>
   <cols>
-    <col min="1" max="1" width="37.5714285714286" customWidth="1"/>
-    <col min="2" max="2" width="9.85714285714286" customWidth="1"/>
-    <col min="3" max="3" width="8.85714285714286" customWidth="1"/>
-    <col min="4" max="4" width="14" customWidth="1"/>
-    <col min="5" max="5" width="89.2857142857143" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="37.5714285714286" collapsed="false"/>
+    <col min="2" max="2" customWidth="true" width="9.85714285714286" collapsed="false"/>
+    <col min="3" max="3" customWidth="true" width="8.85714285714286" collapsed="false"/>
+    <col min="4" max="4" customWidth="true" width="14.0" collapsed="false"/>
+    <col min="5" max="5" customWidth="true" width="89.2857142857143" collapsed="false"/>
   </cols>
   <sheetData>
-    <row r="1" ht="30" spans="1:5">
+    <row ht="30" r="1" spans="1:5">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -1331,10 +1567,18 @@
       <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="2"/>
+      <c r="B2" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>89</v>
+      </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="2" t="s">
@@ -1349,93 +1593,157 @@
       <c r="A4" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="2"/>
+      <c r="B4" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>93</v>
+      </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="2"/>
+      <c r="B5" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>97</v>
+      </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="2"/>
+      <c r="B6" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="2"/>
+      <c r="B7" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>105</v>
+      </c>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="3"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="2"/>
+      <c r="B8" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>109</v>
+      </c>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="3"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="2"/>
+      <c r="B9" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B10" s="3"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="2"/>
+      <c r="B10" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>117</v>
+      </c>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B11" s="3"/>
-      <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
-      <c r="E11" s="2"/>
+      <c r="B11" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>121</v>
+      </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
+  <pageMargins bottom="1" footer="0.511805555555556" header="0.511805555555556" left="0.75" right="0.75" top="1"/>
   <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <sheetPr/>
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1:C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="7" outlineLevelCol="3"/>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="3" outlineLevelRow="7"/>
   <cols>
-    <col min="1" max="1" width="37.5714285714286" customWidth="1"/>
-    <col min="3" max="3" width="12.2857142857143" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="37.5714285714286" collapsed="false"/>
+    <col min="3" max="3" customWidth="true" width="12.2857142857143" collapsed="false"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -1453,8 +1761,12 @@
       <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
+      <c r="B2" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>54</v>
+      </c>
       <c r="D2" t="s">
         <v>19</v>
       </c>
@@ -1463,8 +1775,12 @@
       <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="4"/>
-      <c r="C3" s="4"/>
+      <c r="B3" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>56</v>
+      </c>
       <c r="D3" t="s">
         <v>19</v>
       </c>
@@ -1473,47 +1789,67 @@
       <c r="A4" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="4"/>
-      <c r="C4" s="4"/>
+      <c r="B4" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="4"/>
-      <c r="C5" s="4"/>
+      <c r="B5" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>60</v>
+      </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="5"/>
-      <c r="C6" s="4"/>
+      <c r="B6" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
+      <c r="B7" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B8" s="3"/>
-      <c r="C8" s="3"/>
+      <c r="B8" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>66</v>
+      </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
+  <pageMargins bottom="1" footer="0.511805555555556" header="0.511805555555556" left="0.75" right="0.75" top="1"/>
   <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <sheetPr/>
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2:B11"/>
@@ -1521,8 +1857,8 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="1"/>
   <cols>
-    <col min="1" max="1" width="37.5714285714286" customWidth="1"/>
-    <col min="2" max="2" width="13.2857142857143" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="37.5714285714286" collapsed="false"/>
+    <col min="2" max="2" customWidth="true" width="13.2857142857143" collapsed="false"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -1594,15 +1930,15 @@
       <c r="B11" s="3"/>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
+  <pageMargins bottom="1" footer="0.511805555555556" header="0.511805555555556" left="0.75" right="0.75" top="1"/>
   <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <sheetPr/>
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1:A9"/>
@@ -1610,13 +1946,13 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="3"/>
   <cols>
-    <col min="1" max="1" width="37.5714285714286" customWidth="1"/>
-    <col min="2" max="2" width="12.2857142857143" customWidth="1"/>
-    <col min="3" max="3" width="11.1428571428571" customWidth="1"/>
-    <col min="4" max="4" width="65" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="37.5714285714286" collapsed="false"/>
+    <col min="2" max="2" customWidth="true" width="12.2857142857143" collapsed="false"/>
+    <col min="3" max="3" customWidth="true" width="11.1428571428571" collapsed="false"/>
+    <col min="4" max="4" customWidth="true" width="65.0" collapsed="false"/>
   </cols>
   <sheetData>
-    <row r="1" ht="21" customHeight="1" spans="1:4">
+    <row customHeight="1" ht="21" r="1" spans="1:4">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -1641,7 +1977,7 @@
         <v>25</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>26</v>
+        <v>67</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -1655,7 +1991,7 @@
         <v>28</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>29</v>
+        <v>68</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -1663,13 +1999,13 @@
         <v>5</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>31</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>32</v>
+        <v>69</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -1683,7 +2019,7 @@
         <v>25</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>34</v>
+        <v>70</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -1691,13 +2027,13 @@
         <v>7</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>35</v>
+        <v>72</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>36</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>37</v>
+        <v>71</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -1711,7 +2047,7 @@
         <v>39</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>40</v>
+        <v>73</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -1725,7 +2061,7 @@
         <v>42</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>43</v>
+        <v>74</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -1739,7 +2075,7 @@
         <v>44</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>45</v>
+        <v>75</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -1747,13 +2083,13 @@
         <v>11</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>46</v>
+        <v>77</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>47</v>
       </c>
       <c r="D10" s="7" t="s">
-        <v>48</v>
+        <v>76</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -1761,35 +2097,35 @@
         <v>12</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>25</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>50</v>
+        <v>78</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
+  <pageMargins bottom="1" footer="0.511805555555556" header="0.511805555555556" left="0.75" right="0.75" top="1"/>
   <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <sheetPr/>
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="7" outlineLevelCol="2"/>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="2" outlineLevelRow="7"/>
   <cols>
-    <col min="1" max="1" width="37.5714285714286" customWidth="1"/>
-    <col min="2" max="2" width="6.28571428571429" customWidth="1"/>
-    <col min="3" max="3" width="8.71428571428571" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="37.5714285714286" collapsed="false"/>
+    <col min="2" max="2" customWidth="true" width="6.28571428571429" collapsed="false"/>
+    <col min="3" max="3" customWidth="true" width="8.71428571428571" collapsed="false"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -1853,7 +2189,7 @@
       <c r="C8" s="3"/>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
+  <pageMargins bottom="1" footer="0.511805555555556" header="0.511805555555556" left="0.75" right="0.75" top="1"/>
   <headerFooter/>
 </worksheet>
 </file>
</xml_diff>